<commit_message>
Traduzido bg13 até a linha 450.
</commit_message>
<xml_diff>
--- a/glossario.xlsx
+++ b/glossario.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moacyr\Desktop\GITHUB-BD\traducao-blue-dragon-xbox360\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\danger\traducoes\traducao-blue-dragon-xbox360\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>Aerial Troop</t>
   </si>
@@ -93,6 +93,18 @@
   </si>
   <si>
     <t>máquina de perfuração</t>
+  </si>
+  <si>
+    <t>Blademasters</t>
+  </si>
+  <si>
+    <t>Mestres da Espada</t>
+  </si>
+  <si>
+    <t>purple cloud</t>
+  </si>
+  <si>
+    <t>nuvem roxa</t>
   </si>
 </sst>
 </file>
@@ -416,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E11"/>
+  <dimension ref="B1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -522,6 +534,22 @@
         <v>22</v>
       </c>
     </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Ajustada tools e glossario.xlsx
</commit_message>
<xml_diff>
--- a/glossario.xlsx
+++ b/glossario.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="130">
   <si>
     <t>Aerial Troop</t>
   </si>
@@ -269,9 +269,6 @@
     <t>Flara</t>
   </si>
   <si>
-    <t>Fogo</t>
-  </si>
-  <si>
     <t>Flare</t>
   </si>
   <si>
@@ -326,18 +323,6 @@
     <t>nocaute</t>
   </si>
   <si>
-    <t>Fogo2</t>
-  </si>
-  <si>
-    <t>Fogo3</t>
-  </si>
-  <si>
-    <t>Terra2</t>
-  </si>
-  <si>
-    <t>Terra3</t>
-  </si>
-  <si>
     <t>Shadow</t>
   </si>
   <si>
@@ -350,12 +335,6 @@
     <t>Sombra</t>
   </si>
   <si>
-    <t>Sombra2</t>
-  </si>
-  <si>
-    <t>Sombra3</t>
-  </si>
-  <si>
     <t>Shina</t>
   </si>
   <si>
@@ -365,9 +344,6 @@
     <t>Luz</t>
   </si>
   <si>
-    <t>Luz2</t>
-  </si>
-  <si>
     <t>Water</t>
   </si>
   <si>
@@ -380,12 +356,6 @@
     <t>Água</t>
   </si>
   <si>
-    <t>Água2</t>
-  </si>
-  <si>
-    <t>Água3</t>
-  </si>
-  <si>
     <t>Wind</t>
   </si>
   <si>
@@ -398,12 +368,6 @@
     <t>Vento</t>
   </si>
   <si>
-    <t>Vento2</t>
-  </si>
-  <si>
-    <t>Vento3</t>
-  </si>
-  <si>
     <t>Magias</t>
   </si>
   <si>
@@ -416,7 +380,40 @@
     <t>Erase</t>
   </si>
   <si>
-    <t>Dissolução</t>
+    <t>Chama</t>
+  </si>
+  <si>
+    <t>Chamae</t>
+  </si>
+  <si>
+    <t>Terrae</t>
+  </si>
+  <si>
+    <t>Sombrae</t>
+  </si>
+  <si>
+    <t>Luze</t>
+  </si>
+  <si>
+    <t>Terraus</t>
+  </si>
+  <si>
+    <t>Chamaus</t>
+  </si>
+  <si>
+    <t>Sombraus</t>
+  </si>
+  <si>
+    <t>Ventoe</t>
+  </si>
+  <si>
+    <t>Vetous</t>
+  </si>
+  <si>
+    <t>Aguae</t>
+  </si>
+  <si>
+    <t>Aguaus</t>
   </si>
 </sst>
 </file>
@@ -760,19 +757,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C70" sqref="C70"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="19.5703125" customWidth="1"/>
-    <col min="3" max="3" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="C1" s="2"/>
     </row>
@@ -888,7 +885,7 @@
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="C16" s="2"/>
     </row>
@@ -1111,56 +1108,56 @@
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B46" s="2" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="C46" s="2"/>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
+        <v>87</v>
+      </c>
+      <c r="C47" t="s">
         <v>88</v>
-      </c>
-      <c r="C47" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
+        <v>89</v>
+      </c>
+      <c r="C48" t="s">
         <v>90</v>
-      </c>
-      <c r="C48" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
+        <v>91</v>
+      </c>
+      <c r="C49" t="s">
         <v>92</v>
-      </c>
-      <c r="C49" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
+        <v>93</v>
+      </c>
+      <c r="C50" t="s">
         <v>94</v>
-      </c>
-      <c r="C50" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
+        <v>95</v>
+      </c>
+      <c r="C51" t="s">
         <v>96</v>
-      </c>
-      <c r="C51" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
+        <v>97</v>
+      </c>
+      <c r="C52" t="s">
         <v>98</v>
-      </c>
-      <c r="C52" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.25">
@@ -1168,143 +1165,140 @@
         <v>80</v>
       </c>
       <c r="C53" t="s">
-        <v>81</v>
+        <v>118</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C54" t="s">
-        <v>100</v>
+        <v>119</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C55" t="s">
-        <v>101</v>
+        <v>124</v>
       </c>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
+        <v>83</v>
+      </c>
+      <c r="C56" t="s">
         <v>84</v>
-      </c>
-      <c r="C56" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C57" t="s">
-        <v>102</v>
+        <v>120</v>
       </c>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C58" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C59" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C60" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C61" t="s">
-        <v>109</v>
+        <v>125</v>
       </c>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="C62" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
     </row>
     <row r="63" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="C63" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C64" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C65" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="C66" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="C67" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="C68" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="C69" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>129</v>
-      </c>
-      <c r="C70" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Criada abas para glossario.xlsx
</commit_message>
<xml_diff>
--- a/glossario.xlsx
+++ b/glossario.xlsx
@@ -9,12 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="Diversos" sheetId="2" r:id="rId1"/>
+    <sheet name="Pedras e Joias" sheetId="5" r:id="rId2"/>
+    <sheet name="Lugares" sheetId="4" r:id="rId3"/>
+    <sheet name="Magias" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="160">
   <si>
     <t>Aerial Troop</t>
   </si>
@@ -299,15 +303,9 @@
     <t>enfermidades</t>
   </si>
   <si>
-    <t>Dark (magia)</t>
-  </si>
-  <si>
     <t>Escuridão</t>
   </si>
   <si>
-    <t>dizzy (magia)</t>
-  </si>
-  <si>
     <t>Vertigem</t>
   </si>
   <si>
@@ -414,6 +412,102 @@
   </si>
   <si>
     <t>Aguaus</t>
+  </si>
+  <si>
+    <t>Dissolução</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dark </t>
+  </si>
+  <si>
+    <t>Dizzy</t>
+  </si>
+  <si>
+    <t>Pedras e Jóias</t>
+  </si>
+  <si>
+    <t>Mad Amethyst</t>
+  </si>
+  <si>
+    <t>Ametista Louca</t>
+  </si>
+  <si>
+    <t>White Diamond</t>
+  </si>
+  <si>
+    <t>Diamante Branco</t>
+  </si>
+  <si>
+    <t>Angel's Emerald</t>
+  </si>
+  <si>
+    <t>Esmeralda do Anjo</t>
+  </si>
+  <si>
+    <t>Princess Garnet</t>
+  </si>
+  <si>
+    <t>Granada da Princesa</t>
+  </si>
+  <si>
+    <t>Spiritual Moon</t>
+  </si>
+  <si>
+    <t>Lua Espiritual</t>
+  </si>
+  <si>
+    <t>Base Stone</t>
+  </si>
+  <si>
+    <t>Pedra Base</t>
+  </si>
+  <si>
+    <t>Small Opal</t>
+  </si>
+  <si>
+    <t>Pequena Opala</t>
+  </si>
+  <si>
+    <t>Silent Peridot</t>
+  </si>
+  <si>
+    <t>Peridoto Silencioso</t>
+  </si>
+  <si>
+    <t>Leaf Ruby</t>
+  </si>
+  <si>
+    <t>Rubi de Folha</t>
+  </si>
+  <si>
+    <t>Ocean Topaz</t>
+  </si>
+  <si>
+    <t>Topázio do Oceano</t>
+  </si>
+  <si>
+    <t>Star Tourmaline</t>
+  </si>
+  <si>
+    <t>Turmalina da Estrela</t>
+  </si>
+  <si>
+    <t>Turquoise of Love</t>
+  </si>
+  <si>
+    <t>Turquesa do Amor</t>
+  </si>
+  <si>
+    <t>Black Zircon</t>
+  </si>
+  <si>
+    <t>Zircônio Negro</t>
+  </si>
+  <si>
+    <t>Red Onyx</t>
+  </si>
+  <si>
+    <t>Ônix Vermelho</t>
   </si>
 </sst>
 </file>
@@ -755,10 +849,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E70"/>
+  <dimension ref="B1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B42" sqref="B42:C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -769,7 +863,7 @@
   <sheetData>
     <row r="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C1" s="2"/>
     </row>
@@ -883,431 +977,645 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="C16" s="2"/>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C17" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>31</v>
-      </c>
-      <c r="C19" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>33</v>
-      </c>
-      <c r="C20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>34</v>
-      </c>
-      <c r="C21" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C22" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>39</v>
-      </c>
-      <c r="C23" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>41</v>
-      </c>
-      <c r="C25" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>42</v>
-      </c>
-      <c r="C26" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>46</v>
-      </c>
-      <c r="C27" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>48</v>
-      </c>
-      <c r="C28" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>50</v>
-      </c>
-      <c r="C29" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>51</v>
-      </c>
-      <c r="C30" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>54</v>
-      </c>
-      <c r="C31" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>56</v>
-      </c>
-      <c r="C32" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>58</v>
-      </c>
-      <c r="C33" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>59</v>
-      </c>
-      <c r="C34" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>62</v>
-      </c>
-      <c r="C35" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>64</v>
-      </c>
-      <c r="C36" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
-        <v>66</v>
-      </c>
-      <c r="C37" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>67</v>
-      </c>
-      <c r="C38" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>70</v>
-      </c>
-      <c r="C39" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
-        <v>72</v>
-      </c>
-      <c r="C40" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
-        <v>74</v>
-      </c>
-      <c r="C42" t="s">
-        <v>75</v>
-      </c>
+    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D42" s="1"/>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
-        <v>76</v>
-      </c>
-      <c r="C43" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
-        <v>78</v>
-      </c>
-      <c r="C44" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B46" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C46" s="2"/>
-    </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
-        <v>87</v>
-      </c>
-      <c r="C47" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
-        <v>89</v>
-      </c>
-      <c r="C48" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
-        <v>91</v>
-      </c>
-      <c r="C49" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
-        <v>93</v>
-      </c>
-      <c r="C50" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
-        <v>95</v>
-      </c>
-      <c r="C51" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
-        <v>97</v>
-      </c>
-      <c r="C52" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
-        <v>80</v>
-      </c>
-      <c r="C53" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
-        <v>81</v>
-      </c>
-      <c r="C54" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
-        <v>82</v>
-      </c>
-      <c r="C55" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B56" t="s">
-        <v>83</v>
-      </c>
-      <c r="C56" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
-        <v>85</v>
-      </c>
-      <c r="C57" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B58" t="s">
-        <v>86</v>
-      </c>
-      <c r="C58" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B59" t="s">
-        <v>99</v>
-      </c>
-      <c r="C59" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B60" t="s">
-        <v>100</v>
-      </c>
-      <c r="C60" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B61" t="s">
-        <v>101</v>
-      </c>
-      <c r="C61" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B62" t="s">
-        <v>103</v>
-      </c>
-      <c r="C62" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B63" t="s">
-        <v>104</v>
-      </c>
-      <c r="C63" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B64" t="s">
-        <v>106</v>
-      </c>
-      <c r="C64" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B65" t="s">
-        <v>107</v>
-      </c>
-      <c r="C65" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B66" t="s">
-        <v>108</v>
-      </c>
-      <c r="C66" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B67" t="s">
-        <v>110</v>
-      </c>
-      <c r="C67" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B68" t="s">
-        <v>111</v>
-      </c>
-      <c r="C68" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B69" t="s">
-        <v>112</v>
-      </c>
-      <c r="C69" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B70" t="s">
-        <v>117</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B16:C16"/>
+  <mergeCells count="1">
     <mergeCell ref="B1:C1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:C20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C4" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>156</v>
+      </c>
+      <c r="C5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>148</v>
+      </c>
+      <c r="C10" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>132</v>
+      </c>
+      <c r="C11" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>150</v>
+      </c>
+      <c r="C12" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>138</v>
+      </c>
+      <c r="C13" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>158</v>
+      </c>
+      <c r="C14" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>146</v>
+      </c>
+      <c r="C15" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>144</v>
+      </c>
+      <c r="C16" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>140</v>
+      </c>
+      <c r="C17" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>152</v>
+      </c>
+      <c r="C18" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>154</v>
+      </c>
+      <c r="C19" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>134</v>
+      </c>
+      <c r="C20" t="s">
+        <v>135</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="B2:C20">
+    <sortCondition ref="B2"/>
+  </sortState>
+  <mergeCells count="1">
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:D25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>64</v>
+      </c>
+      <c r="C21" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>70</v>
+      </c>
+      <c r="C24" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>72</v>
+      </c>
+      <c r="C25" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="B2:C25">
+    <sortCondition ref="B2"/>
+  </sortState>
+  <mergeCells count="1">
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:C25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C6" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C9" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C10" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>95</v>
+      </c>
+      <c r="C11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>87</v>
+      </c>
+      <c r="C12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>97</v>
+      </c>
+      <c r="C13" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>98</v>
+      </c>
+      <c r="C14" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>99</v>
+      </c>
+      <c r="C15" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>101</v>
+      </c>
+      <c r="C16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>102</v>
+      </c>
+      <c r="C17" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>93</v>
+      </c>
+      <c r="C18" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>89</v>
+      </c>
+      <c r="C19" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>104</v>
+      </c>
+      <c r="C20" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>105</v>
+      </c>
+      <c r="C21" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>106</v>
+      </c>
+      <c r="C22" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>108</v>
+      </c>
+      <c r="C23" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>109</v>
+      </c>
+      <c r="C24" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>110</v>
+      </c>
+      <c r="C25" t="s">
+        <v>125</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="B2:C25">
+    <sortCondition ref="B2"/>
+  </sortState>
+  <mergeCells count="1">
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Traduzido da linha 1712 até o fim do SkWd_new_us.u16 Atualizado o glossário com nomes de magias.
</commit_message>
<xml_diff>
--- a/glossario.xlsx
+++ b/glossario.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Diversos" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,6 @@
     <sheet name="Magias" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="242">
   <si>
     <t>Aerial Troop</t>
   </si>
@@ -309,9 +308,6 @@
     <t>Vertigem</t>
   </si>
   <si>
-    <t>Sleep(magia)</t>
-  </si>
-  <si>
     <t>Sono</t>
   </si>
   <si>
@@ -390,9 +386,6 @@
     <t>Sombrae</t>
   </si>
   <si>
-    <t>Luze</t>
-  </si>
-  <si>
     <t>Terraus</t>
   </si>
   <si>
@@ -508,6 +501,258 @@
   </si>
   <si>
     <t>Ônix Vermelho</t>
+  </si>
+  <si>
+    <t>Wall</t>
+  </si>
+  <si>
+    <t>Walla</t>
+  </si>
+  <si>
+    <t>Wallus</t>
+  </si>
+  <si>
+    <t>Muralha</t>
+  </si>
+  <si>
+    <t>Muralhae</t>
+  </si>
+  <si>
+    <t>Muralhaus</t>
+  </si>
+  <si>
+    <t>Resist</t>
+  </si>
+  <si>
+    <t>Resista</t>
+  </si>
+  <si>
+    <t>Resistus</t>
+  </si>
+  <si>
+    <t>Poison</t>
+  </si>
+  <si>
+    <t>Imune</t>
+  </si>
+  <si>
+    <t>Imuna</t>
+  </si>
+  <si>
+    <t>Panic</t>
+  </si>
+  <si>
+    <t>Pânico</t>
+  </si>
+  <si>
+    <t>Petrify</t>
+  </si>
+  <si>
+    <t>Petrificação</t>
+  </si>
+  <si>
+    <t>Imunus</t>
+  </si>
+  <si>
+    <t>Sleep</t>
+  </si>
+  <si>
+    <t>Trapfloor</t>
+  </si>
+  <si>
+    <t>Trapfloora</t>
+  </si>
+  <si>
+    <t>Trapfloorus</t>
+  </si>
+  <si>
+    <t>Armadilha</t>
+  </si>
+  <si>
+    <t>Armadilhae</t>
+  </si>
+  <si>
+    <t>Armadilhaus</t>
+  </si>
+  <si>
+    <t>Reflect</t>
+  </si>
+  <si>
+    <t>Reflecta</t>
+  </si>
+  <si>
+    <t>Reflexo</t>
+  </si>
+  <si>
+    <t>Reflexa</t>
+  </si>
+  <si>
+    <t>Shell</t>
+  </si>
+  <si>
+    <t>Shella</t>
+  </si>
+  <si>
+    <t>Shellus</t>
+  </si>
+  <si>
+    <t>Carapaçae</t>
+  </si>
+  <si>
+    <t>Carapaça</t>
+  </si>
+  <si>
+    <t>Carapaçaus</t>
+  </si>
+  <si>
+    <t>Shield</t>
+  </si>
+  <si>
+    <t>Shielda</t>
+  </si>
+  <si>
+    <t>Shieldus</t>
+  </si>
+  <si>
+    <t>Escudous</t>
+  </si>
+  <si>
+    <t>Escudo</t>
+  </si>
+  <si>
+    <t>Escuda</t>
+  </si>
+  <si>
+    <t>Deflect</t>
+  </si>
+  <si>
+    <t>Acurácia</t>
+  </si>
+  <si>
+    <t>Curse</t>
+  </si>
+  <si>
+    <t>Maldição</t>
+  </si>
+  <si>
+    <t>Quick</t>
+  </si>
+  <si>
+    <t>Quicka</t>
+  </si>
+  <si>
+    <t>Quickus</t>
+  </si>
+  <si>
+    <t>Rapidez</t>
+  </si>
+  <si>
+    <t>Rapideze</t>
+  </si>
+  <si>
+    <t>Rapidezus</t>
+  </si>
+  <si>
+    <t>Slow</t>
+  </si>
+  <si>
+    <t>Slowa</t>
+  </si>
+  <si>
+    <t>Slowus</t>
+  </si>
+  <si>
+    <t>Lentidão</t>
+  </si>
+  <si>
+    <t>Lentidãoe</t>
+  </si>
+  <si>
+    <t>Lentidãous</t>
+  </si>
+  <si>
+    <t>Extract</t>
+  </si>
+  <si>
+    <t>Extracta</t>
+  </si>
+  <si>
+    <t>Extractus</t>
+  </si>
+  <si>
+    <t>Absorção</t>
+  </si>
+  <si>
+    <t>Absorçãoe</t>
+  </si>
+  <si>
+    <t>Absorçãous</t>
+  </si>
+  <si>
+    <t>Luza</t>
+  </si>
+  <si>
+    <t>Cancel</t>
+  </si>
+  <si>
+    <t>Anulação</t>
+  </si>
+  <si>
+    <t>Regenerate</t>
+  </si>
+  <si>
+    <t>Regeneração</t>
+  </si>
+  <si>
+    <t>Regeneraçãoe</t>
+  </si>
+  <si>
+    <t>Regenera</t>
+  </si>
+  <si>
+    <t>Revive</t>
+  </si>
+  <si>
+    <t>Previve</t>
+  </si>
+  <si>
+    <t>Auto-Revive</t>
+  </si>
+  <si>
+    <t>Zephyrus</t>
+  </si>
+  <si>
+    <t>Zephyr</t>
+  </si>
+  <si>
+    <t>Zephyra</t>
+  </si>
+  <si>
+    <t>Vitalidade</t>
+  </si>
+  <si>
+    <t>Vitalidadea</t>
+  </si>
+  <si>
+    <t>Vitalidadeus</t>
+  </si>
+  <si>
+    <t>Heal</t>
+  </si>
+  <si>
+    <t>Heala</t>
+  </si>
+  <si>
+    <t>Healus</t>
+  </si>
+  <si>
+    <t>Cura</t>
+  </si>
+  <si>
+    <t>Curae</t>
+  </si>
+  <si>
+    <t>Curaus</t>
   </si>
 </sst>
 </file>
@@ -557,9 +802,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -862,10 +1108,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C1" s="2"/>
+      <c r="B1" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C1" s="3"/>
     </row>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -993,7 +1239,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
@@ -1004,17 +1250,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="C1" s="2"/>
+      <c r="B1" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C1" s="3"/>
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
@@ -1027,18 +1273,18 @@
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
@@ -1075,90 +1321,90 @@
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C10" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C11" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C12" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C13" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C15" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C16" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C17" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C18" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C19" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C20" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -1187,10 +1433,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="C1" s="2"/>
+      <c r="B1" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C1" s="3"/>
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -1399,10 +1645,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:C25"/>
+  <dimension ref="B1:G67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1412,210 +1658,549 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C1" s="2"/>
+      <c r="B1" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" s="3"/>
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>129</v>
+        <v>221</v>
       </c>
       <c r="C2" t="s">
-        <v>91</v>
+        <v>222</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>130</v>
+        <v>200</v>
       </c>
       <c r="C3" t="s">
-        <v>92</v>
+        <v>201</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>115</v>
+        <v>127</v>
       </c>
       <c r="C4" t="s">
-        <v>128</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>80</v>
+        <v>198</v>
       </c>
       <c r="C5" t="s">
-        <v>116</v>
+        <v>199</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>81</v>
+        <v>128</v>
       </c>
       <c r="C6" t="s">
-        <v>117</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>82</v>
+        <v>114</v>
       </c>
       <c r="C7" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>83</v>
+        <v>214</v>
       </c>
       <c r="C8" t="s">
-        <v>84</v>
+        <v>217</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>85</v>
+        <v>215</v>
       </c>
       <c r="C9" t="s">
-        <v>118</v>
+        <v>218</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>86</v>
+        <v>216</v>
       </c>
       <c r="C10" t="s">
-        <v>121</v>
+        <v>219</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="C11" t="s">
-        <v>96</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C12" t="s">
-        <v>88</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="C13" t="s">
-        <v>100</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="C14" t="s">
-        <v>119</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="C15" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
+        <v>86</v>
+      </c>
+      <c r="C16" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>236</v>
+      </c>
+      <c r="C17" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>237</v>
+      </c>
+      <c r="C18" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>238</v>
+      </c>
+      <c r="C19" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>94</v>
+      </c>
+      <c r="C20" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>170</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>87</v>
+      </c>
+      <c r="C22" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>172</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="G23" s="2"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>228</v>
+      </c>
+      <c r="C25" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>202</v>
+      </c>
+      <c r="C26" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>203</v>
+      </c>
+      <c r="C27" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>204</v>
+      </c>
+      <c r="C28" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>182</v>
+      </c>
+      <c r="C29" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>183</v>
+      </c>
+      <c r="C30" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>226</v>
+      </c>
+      <c r="C31" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>223</v>
+      </c>
+      <c r="C32" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>164</v>
+      </c>
+      <c r="C33" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>165</v>
+      </c>
+      <c r="C34" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C35" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>227</v>
+      </c>
+      <c r="C36" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>96</v>
+      </c>
+      <c r="C37" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>97</v>
+      </c>
+      <c r="C38" t="s">
+        <v>118</v>
+      </c>
+      <c r="F38" s="1"/>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>98</v>
+      </c>
+      <c r="C39" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>186</v>
+      </c>
+      <c r="C40" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>187</v>
+      </c>
+      <c r="C41" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>188</v>
+      </c>
+      <c r="C42" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>192</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>193</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>194</v>
+      </c>
+      <c r="C45" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>100</v>
+      </c>
+      <c r="C46" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
         <v>101</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C47" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>175</v>
+      </c>
+      <c r="C48" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>208</v>
+      </c>
+      <c r="C49" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>209</v>
+      </c>
+      <c r="C50" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>210</v>
+      </c>
+      <c r="C51" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>89</v>
+      </c>
+      <c r="C52" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>176</v>
+      </c>
+      <c r="C53" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>177</v>
+      </c>
+      <c r="C54" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>178</v>
+      </c>
+      <c r="C55" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>158</v>
+      </c>
+      <c r="C56" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>159</v>
+      </c>
+      <c r="C57" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>160</v>
+      </c>
+      <c r="C58" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>102</v>
-      </c>
-      <c r="C17" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>93</v>
-      </c>
-      <c r="C18" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>89</v>
-      </c>
-      <c r="C19" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
+      <c r="C59" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
         <v>104</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C60" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>105</v>
+      </c>
+      <c r="C61" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>105</v>
-      </c>
-      <c r="C21" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>106</v>
-      </c>
-      <c r="C22" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+      <c r="C62" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
         <v>108</v>
       </c>
-      <c r="C23" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
+      <c r="C63" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
         <v>109</v>
       </c>
-      <c r="C24" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>110</v>
-      </c>
-      <c r="C25" t="s">
-        <v>125</v>
+      <c r="C64" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>231</v>
+      </c>
+      <c r="C65" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>232</v>
+      </c>
+      <c r="C66" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>230</v>
+      </c>
+      <c r="C67" t="s">
+        <v>235</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="B2:C25">
+  <sortState ref="B2:C67">
     <sortCondition ref="B2"/>
   </sortState>
   <mergeCells count="1">
     <mergeCell ref="B1:C1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Traduzidas primeiras 300 linhas do SkWd_new_us.u16
</commit_message>
<xml_diff>
--- a/glossario.xlsx
+++ b/glossario.xlsx
@@ -5,17 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moacyr\Desktop\GITHUB-BLUE DRAGON\traducao-blue-dragon-xbox360\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\danger\traducoes\traducao-blue-dragon-xbox360\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Diversos" sheetId="2" r:id="rId1"/>
     <sheet name="Pedras e Joias" sheetId="5" r:id="rId2"/>
     <sheet name="Lugares" sheetId="4" r:id="rId3"/>
     <sheet name="Magias" sheetId="3" r:id="rId4"/>
+    <sheet name="Ações" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="316">
   <si>
     <t>Aerial Troop</t>
   </si>
@@ -759,6 +760,222 @@
   </si>
   <si>
     <t>Excluido</t>
+  </si>
+  <si>
+    <t>Double Shot</t>
+  </si>
+  <si>
+    <t>Disparo Duplo</t>
+  </si>
+  <si>
+    <t>Szabo Spin</t>
+  </si>
+  <si>
+    <t>Giro de Szabo</t>
+  </si>
+  <si>
+    <t>Putrefaction Gas</t>
+  </si>
+  <si>
+    <t>Gás Tóxico</t>
+  </si>
+  <si>
+    <t>Crimson Blood Rain</t>
+  </si>
+  <si>
+    <t>Chuva de Sangue Carmesim</t>
+  </si>
+  <si>
+    <t>Everyone's Enmity</t>
+  </si>
+  <si>
+    <t>Inimizade de Todos</t>
+  </si>
+  <si>
+    <t>Bullish Mode</t>
+  </si>
+  <si>
+    <t>Modo Intimidador</t>
+  </si>
+  <si>
+    <t>Final Summons</t>
+  </si>
+  <si>
+    <t>Invocação Final</t>
+  </si>
+  <si>
+    <t>Mist Consumption</t>
+  </si>
+  <si>
+    <t>Consumo de Neblina</t>
+  </si>
+  <si>
+    <t>Stop Absorption</t>
+  </si>
+  <si>
+    <t>Parar Absorção</t>
+  </si>
+  <si>
+    <t>Marble Storm</t>
+  </si>
+  <si>
+    <t>Tormenta de Mármore</t>
+  </si>
+  <si>
+    <t>Licking Lips</t>
+  </si>
+  <si>
+    <t>Lambendo Lábios</t>
+  </si>
+  <si>
+    <t>Light Counterattack</t>
+  </si>
+  <si>
+    <t>Contra-ataque ligeiro</t>
+  </si>
+  <si>
+    <t>Smoke Suction</t>
+  </si>
+  <si>
+    <t>Sucção de Fumaça</t>
+  </si>
+  <si>
+    <t>Primitive Fire</t>
+  </si>
+  <si>
+    <t>Fogo Primitivo</t>
+  </si>
+  <si>
+    <t>Forced Death</t>
+  </si>
+  <si>
+    <t>Morte Forçada</t>
+  </si>
+  <si>
+    <t>Mecha Robo</t>
+  </si>
+  <si>
+    <t>robô mecanóide</t>
+  </si>
+  <si>
+    <t>Dragon Roar</t>
+  </si>
+  <si>
+    <t>Rugido de Dragão</t>
+  </si>
+  <si>
+    <t>Wind Gun</t>
+  </si>
+  <si>
+    <t>Canhão de Vento</t>
+  </si>
+  <si>
+    <t>Earth Gun</t>
+  </si>
+  <si>
+    <t>Canhão de Terra</t>
+  </si>
+  <si>
+    <t>Death Blossom</t>
+  </si>
+  <si>
+    <t>Flor da Morte</t>
+  </si>
+  <si>
+    <t>One Hundred Venomous Roots</t>
+  </si>
+  <si>
+    <t>Cem raízes venenosas</t>
+  </si>
+  <si>
+    <t>Stone Sap</t>
+  </si>
+  <si>
+    <t>Seiva de Pedra</t>
+  </si>
+  <si>
+    <t>Final Judgment</t>
+  </si>
+  <si>
+    <t>Juízo Final</t>
+  </si>
+  <si>
+    <t>Energy Blast</t>
+  </si>
+  <si>
+    <t>Rajada de Energia</t>
+  </si>
+  <si>
+    <t>Loud Laugh</t>
+  </si>
+  <si>
+    <t>Gargalhada</t>
+  </si>
+  <si>
+    <t>Greedy Mist</t>
+  </si>
+  <si>
+    <t>Névoa avarenta</t>
+  </si>
+  <si>
+    <t>Brimstone</t>
+  </si>
+  <si>
+    <t>enxofre</t>
+  </si>
+  <si>
+    <t>Mist Killer</t>
+  </si>
+  <si>
+    <t>Névoa Assassina</t>
+  </si>
+  <si>
+    <t>Marble Marble</t>
+  </si>
+  <si>
+    <t>Pedra de Mármore</t>
+  </si>
+  <si>
+    <t>Marble</t>
+  </si>
+  <si>
+    <t>Bolas de Gude</t>
+  </si>
+  <si>
+    <t>Hundred Thrust</t>
+  </si>
+  <si>
+    <t>Cem estocadas</t>
+  </si>
+  <si>
+    <t>Szavulcan</t>
+  </si>
+  <si>
+    <t>Szavulcão</t>
+  </si>
+  <si>
+    <t>Ray Beam</t>
+  </si>
+  <si>
+    <t>Feixe de raios</t>
+  </si>
+  <si>
+    <t>Continuous Strike</t>
+  </si>
+  <si>
+    <t>Ataque contínuo</t>
+  </si>
+  <si>
+    <t>Punhalada mental</t>
+  </si>
+  <si>
+    <t>Punhalada Múltipla</t>
+  </si>
+  <si>
+    <t>Foice Veloz</t>
+  </si>
+  <si>
+    <t>Ações</t>
   </si>
 </sst>
 </file>
@@ -1103,8 +1320,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1235,6 +1452,14 @@
       </c>
       <c r="C15" t="s">
         <v>243</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>274</v>
+      </c>
+      <c r="C16" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="42" spans="4:4" x14ac:dyDescent="0.25">
@@ -1662,7 +1887,7 @@
   <dimension ref="B1:G67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B1" sqref="B1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2217,4 +2442,323 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:C37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="C1" s="3"/>
+    </row>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>311</v>
+      </c>
+      <c r="C2" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>296</v>
+      </c>
+      <c r="C3" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>254</v>
+      </c>
+      <c r="C4" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>310</v>
+      </c>
+      <c r="C5" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>250</v>
+      </c>
+      <c r="C6" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>282</v>
+      </c>
+      <c r="C7" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>244</v>
+      </c>
+      <c r="C8" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>276</v>
+      </c>
+      <c r="C9" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>280</v>
+      </c>
+      <c r="C10" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>290</v>
+      </c>
+      <c r="C11" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>252</v>
+      </c>
+      <c r="C12" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>288</v>
+      </c>
+      <c r="C13" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>256</v>
+      </c>
+      <c r="C14" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>272</v>
+      </c>
+      <c r="C15" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>294</v>
+      </c>
+      <c r="C16" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>304</v>
+      </c>
+      <c r="C17" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>264</v>
+      </c>
+      <c r="C18" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>266</v>
+      </c>
+      <c r="C19" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>292</v>
+      </c>
+      <c r="C20" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>302</v>
+      </c>
+      <c r="C21" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>300</v>
+      </c>
+      <c r="C22" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>262</v>
+      </c>
+      <c r="C23" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>258</v>
+      </c>
+      <c r="C24" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>298</v>
+      </c>
+      <c r="C25" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>284</v>
+      </c>
+      <c r="C26" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>270</v>
+      </c>
+      <c r="C27" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>312</v>
+      </c>
+      <c r="C28" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>313</v>
+      </c>
+      <c r="C29" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>248</v>
+      </c>
+      <c r="C30" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>308</v>
+      </c>
+      <c r="C31" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>268</v>
+      </c>
+      <c r="C32" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>286</v>
+      </c>
+      <c r="C33" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>260</v>
+      </c>
+      <c r="C34" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>246</v>
+      </c>
+      <c r="C35" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>306</v>
+      </c>
+      <c r="C36" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>278</v>
+      </c>
+      <c r="C37" t="s">
+        <v>279</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="B2:C37">
+    <sortCondition ref="B2"/>
+  </sortState>
+  <mergeCells count="1">
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Traduzido até linha 410 do SkWd_new_us.u16
</commit_message>
<xml_diff>
--- a/glossario.xlsx
+++ b/glossario.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\danger\traducoes\traducao-blue-dragon-xbox360\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="4"/>
   </bookViews>
@@ -17,6 +12,7 @@
     <sheet name="Lugares" sheetId="4" r:id="rId3"/>
     <sheet name="Magias" sheetId="3" r:id="rId4"/>
     <sheet name="Ações" sheetId="7" r:id="rId5"/>
+    <sheet name="Monstros" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="144525"/>
   <extLst>
@@ -28,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="379">
   <si>
     <t>Aerial Troop</t>
   </si>
@@ -976,6 +972,195 @@
   </si>
   <si>
     <t>Ações</t>
+  </si>
+  <si>
+    <t>Monstros e Bestas</t>
+  </si>
+  <si>
+    <t>Gale Wolf Ghost</t>
+  </si>
+  <si>
+    <t>Lobo Fantasma da Ventania</t>
+  </si>
+  <si>
+    <t>Stone Wolf Ghost</t>
+  </si>
+  <si>
+    <t>Weather Anomaly</t>
+  </si>
+  <si>
+    <t>Anomalia Climática</t>
+  </si>
+  <si>
+    <t>Spinning Shell</t>
+  </si>
+  <si>
+    <t>Carapaça Giratória</t>
+  </si>
+  <si>
+    <t>Shocking Sphere</t>
+  </si>
+  <si>
+    <t>Esfera Chocante</t>
+  </si>
+  <si>
+    <t>Earth Wedge</t>
+  </si>
+  <si>
+    <t>Cunha de Terra</t>
+  </si>
+  <si>
+    <t>Jumbo Mecha Robos</t>
+  </si>
+  <si>
+    <t>robô mecanóide gigante</t>
+  </si>
+  <si>
+    <t>War Mecha Robo</t>
+  </si>
+  <si>
+    <t>robô mecanóide de guerra</t>
+  </si>
+  <si>
+    <t>Lobo Fantasma de Pedra</t>
+  </si>
+  <si>
+    <t>Lost Hurricane</t>
+  </si>
+  <si>
+    <t>Furacão Perdido</t>
+  </si>
+  <si>
+    <t>Mow-Down Beam</t>
+  </si>
+  <si>
+    <t>Feixe ceifador</t>
+  </si>
+  <si>
+    <t>Rapid-Fire Gun</t>
+  </si>
+  <si>
+    <t>Canhão de Fogo Rápido</t>
+  </si>
+  <si>
+    <t>Maxtract</t>
+  </si>
+  <si>
+    <t>Maxtração</t>
+  </si>
+  <si>
+    <t>Frightening Glare</t>
+  </si>
+  <si>
+    <t>Clarão Assustador</t>
+  </si>
+  <si>
+    <t>Super-Strong Punch</t>
+  </si>
+  <si>
+    <t>Soco Super-Forte</t>
+  </si>
+  <si>
+    <t>Chaos Flare</t>
+  </si>
+  <si>
+    <t>Chama do Caos</t>
+  </si>
+  <si>
+    <t>Ice Breath</t>
+  </si>
+  <si>
+    <t>Bafo de Gelo</t>
+  </si>
+  <si>
+    <t>Poison Breath</t>
+  </si>
+  <si>
+    <t>Bafo Venenoso</t>
+  </si>
+  <si>
+    <t>Fire Breath</t>
+  </si>
+  <si>
+    <t>Bafo de Fogo</t>
+  </si>
+  <si>
+    <t>Shocking Breath</t>
+  </si>
+  <si>
+    <t>Bafo Chocante</t>
+  </si>
+  <si>
+    <t>Petrification Breath</t>
+  </si>
+  <si>
+    <t>Bafo Petrificador</t>
+  </si>
+  <si>
+    <t>Mow Down</t>
+  </si>
+  <si>
+    <t>Ceifa</t>
+  </si>
+  <si>
+    <t>Ablaze</t>
+  </si>
+  <si>
+    <t>Incineração</t>
+  </si>
+  <si>
+    <t>Blazing Pillar</t>
+  </si>
+  <si>
+    <t>Coluna Ardente</t>
+  </si>
+  <si>
+    <t>Hind-Leg Kick</t>
+  </si>
+  <si>
+    <t>Coice</t>
+  </si>
+  <si>
+    <t>Stun</t>
+  </si>
+  <si>
+    <t>Tonteia</t>
+  </si>
+  <si>
+    <t>Eye Beam</t>
+  </si>
+  <si>
+    <t>Feixe Ocular</t>
+  </si>
+  <si>
+    <t>Tail Swing</t>
+  </si>
+  <si>
+    <t>Balanço da Cauda</t>
+  </si>
+  <si>
+    <t>Tsunami Omen</t>
+  </si>
+  <si>
+    <t>Pressário de Tsunami</t>
+  </si>
+  <si>
+    <t>Massive Tsunami</t>
+  </si>
+  <si>
+    <t>Grande Tsunami</t>
+  </si>
+  <si>
+    <t>Hand Struck</t>
+  </si>
+  <si>
+    <t>Impacto de mão</t>
+  </si>
+  <si>
+    <t>Sticky Sap</t>
+  </si>
+  <si>
+    <t>Seiva Pegajosa</t>
   </si>
 </sst>
 </file>
@@ -1310,7 +1495,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1321,7 +1506,7 @@
   <dimension ref="B1:E42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B16" sqref="B16:C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1452,14 +1637,6 @@
       </c>
       <c r="C15" t="s">
         <v>243</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>274</v>
-      </c>
-      <c r="C16" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="42" spans="4:4" x14ac:dyDescent="0.25">
@@ -1884,10 +2061,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G67"/>
+  <dimension ref="B1:G68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2430,6 +2607,14 @@
       </c>
       <c r="C67" t="s">
         <v>235</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>365</v>
+      </c>
+      <c r="C68" t="s">
+        <v>366</v>
       </c>
     </row>
   </sheetData>
@@ -2446,10 +2631,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:C37"/>
+  <dimension ref="B1:C63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="B2" sqref="B2:C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2466,294 +2651,502 @@
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>311</v>
+        <v>359</v>
       </c>
       <c r="C2" t="s">
-        <v>312</v>
+        <v>360</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>296</v>
+        <v>311</v>
       </c>
       <c r="C3" t="s">
-        <v>297</v>
+        <v>312</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>254</v>
+        <v>361</v>
       </c>
       <c r="C4" t="s">
-        <v>255</v>
+        <v>362</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
       <c r="C5" t="s">
-        <v>311</v>
+        <v>297</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="C6" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>282</v>
+        <v>345</v>
       </c>
       <c r="C7" t="s">
-        <v>283</v>
+        <v>346</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>244</v>
+        <v>310</v>
       </c>
       <c r="C8" t="s">
-        <v>245</v>
+        <v>311</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>276</v>
+        <v>250</v>
       </c>
       <c r="C9" t="s">
-        <v>277</v>
+        <v>251</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="C10" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>290</v>
+        <v>244</v>
       </c>
       <c r="C11" t="s">
-        <v>291</v>
+        <v>245</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>252</v>
+        <v>276</v>
       </c>
       <c r="C12" t="s">
-        <v>253</v>
+        <v>277</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="C13" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>256</v>
+        <v>326</v>
       </c>
       <c r="C14" t="s">
-        <v>257</v>
+        <v>327</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>272</v>
+        <v>290</v>
       </c>
       <c r="C15" t="s">
-        <v>273</v>
+        <v>291</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>294</v>
+        <v>252</v>
       </c>
       <c r="C16" t="s">
-        <v>295</v>
+        <v>253</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>304</v>
+        <v>367</v>
       </c>
       <c r="C17" t="s">
-        <v>305</v>
+        <v>368</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>264</v>
+        <v>288</v>
       </c>
       <c r="C18" t="s">
-        <v>265</v>
+        <v>289</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
       <c r="C19" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>292</v>
+        <v>351</v>
       </c>
       <c r="C20" t="s">
-        <v>293</v>
+        <v>352</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>302</v>
+        <v>272</v>
       </c>
       <c r="C21" t="s">
-        <v>303</v>
+        <v>273</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>300</v>
+        <v>341</v>
       </c>
       <c r="C22" t="s">
-        <v>301</v>
+        <v>342</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>262</v>
+        <v>294</v>
       </c>
       <c r="C23" t="s">
-        <v>263</v>
+        <v>295</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>258</v>
+        <v>375</v>
       </c>
       <c r="C24" t="s">
-        <v>259</v>
+        <v>376</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>298</v>
+        <v>363</v>
       </c>
       <c r="C25" t="s">
-        <v>299</v>
+        <v>364</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>284</v>
+        <v>304</v>
       </c>
       <c r="C26" t="s">
-        <v>285</v>
+        <v>305</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>270</v>
+        <v>347</v>
       </c>
       <c r="C27" t="s">
-        <v>271</v>
+        <v>348</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>312</v>
+        <v>264</v>
       </c>
       <c r="C28" t="s">
-        <v>313</v>
+        <v>265</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>313</v>
+        <v>266</v>
       </c>
       <c r="C29" t="s">
-        <v>314</v>
+        <v>267</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>248</v>
+        <v>333</v>
       </c>
       <c r="C30" t="s">
-        <v>249</v>
+        <v>334</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>308</v>
+        <v>292</v>
       </c>
       <c r="C31" t="s">
-        <v>309</v>
+        <v>293</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>268</v>
+        <v>302</v>
       </c>
       <c r="C32" t="s">
-        <v>269</v>
+        <v>303</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>286</v>
+        <v>300</v>
       </c>
       <c r="C33" t="s">
-        <v>287</v>
+        <v>301</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="C34" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>246</v>
+        <v>373</v>
       </c>
       <c r="C35" t="s">
-        <v>247</v>
+        <v>374</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>306</v>
+        <v>339</v>
       </c>
       <c r="C36" t="s">
-        <v>307</v>
+        <v>340</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
+        <v>258</v>
+      </c>
+      <c r="C37" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>298</v>
+      </c>
+      <c r="C38" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>357</v>
+      </c>
+      <c r="C39" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>335</v>
+      </c>
+      <c r="C40" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>284</v>
+      </c>
+      <c r="C41" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>355</v>
+      </c>
+      <c r="C42" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>349</v>
+      </c>
+      <c r="C43" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>270</v>
+      </c>
+      <c r="C44" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>312</v>
+      </c>
+      <c r="C45" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>313</v>
+      </c>
+      <c r="C46" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>248</v>
+      </c>
+      <c r="C47" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>337</v>
+      </c>
+      <c r="C48" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>308</v>
+      </c>
+      <c r="C49" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>353</v>
+      </c>
+      <c r="C50" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>324</v>
+      </c>
+      <c r="C51" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>268</v>
+      </c>
+      <c r="C52" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>322</v>
+      </c>
+      <c r="C53" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>377</v>
+      </c>
+      <c r="C54" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>286</v>
+      </c>
+      <c r="C55" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>260</v>
+      </c>
+      <c r="C56" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>343</v>
+      </c>
+      <c r="C57" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>246</v>
+      </c>
+      <c r="C58" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>306</v>
+      </c>
+      <c r="C59" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>369</v>
+      </c>
+      <c r="C60" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>371</v>
+      </c>
+      <c r="C61" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>320</v>
+      </c>
+      <c r="C62" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
         <v>278</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C63" t="s">
         <v>279</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="B2:C37">
+  <sortState ref="B2:C63">
     <sortCondition ref="B2"/>
   </sortState>
   <mergeCells count="1">
@@ -2761,4 +3154,72 @@
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="C1" s="3"/>
+    </row>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>317</v>
+      </c>
+      <c r="C2" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>319</v>
+      </c>
+      <c r="C3" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>274</v>
+      </c>
+      <c r="C4" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>328</v>
+      </c>
+      <c r="C5" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>330</v>
+      </c>
+      <c r="C6" t="s">
+        <v>331</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Traduzido até linha 700 do SkWd_new_us.u16
</commit_message>
<xml_diff>
--- a/glossario.xlsx
+++ b/glossario.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\danger\traducoes\traducao-blue-dragon-xbox360\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Diversos" sheetId="2" r:id="rId1"/>
     <sheet name="Pedras e Joias" sheetId="5" r:id="rId2"/>
     <sheet name="Lugares" sheetId="4" r:id="rId3"/>
     <sheet name="Magias" sheetId="3" r:id="rId4"/>
-    <sheet name="Ações" sheetId="7" r:id="rId5"/>
+    <sheet name="Habilidades" sheetId="7" r:id="rId5"/>
     <sheet name="Monstros" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="144525"/>
@@ -24,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="459">
   <si>
     <t>Aerial Troop</t>
   </si>
@@ -971,9 +976,6 @@
     <t>Foice Veloz</t>
   </si>
   <si>
-    <t>Ações</t>
-  </si>
-  <si>
     <t>Monstros e Bestas</t>
   </si>
   <si>
@@ -1161,6 +1163,249 @@
   </si>
   <si>
     <t>Seiva Pegajosa</t>
+  </si>
+  <si>
+    <t>Dust Blow</t>
+  </si>
+  <si>
+    <t>Golpe de Areia</t>
+  </si>
+  <si>
+    <t>Powerful Cleaning</t>
+  </si>
+  <si>
+    <t>Limpeza Poderosa</t>
+  </si>
+  <si>
+    <t>KO Inferno</t>
+  </si>
+  <si>
+    <t>Nocaute Infernal</t>
+  </si>
+  <si>
+    <t>Jaws Knife</t>
+  </si>
+  <si>
+    <t>Garras de Navalha</t>
+  </si>
+  <si>
+    <t>Nose Machine Gun</t>
+  </si>
+  <si>
+    <t>Metralhadora Frontal</t>
+  </si>
+  <si>
+    <t>Dispel Enchantment</t>
+  </si>
+  <si>
+    <t>Dissipar Feitiço</t>
+  </si>
+  <si>
+    <t>Blizzard</t>
+  </si>
+  <si>
+    <t>Nevasca</t>
+  </si>
+  <si>
+    <t>Prece de Aço</t>
+  </si>
+  <si>
+    <t>Steel Prayer</t>
+  </si>
+  <si>
+    <t>Blast</t>
+  </si>
+  <si>
+    <t>Explosão</t>
+  </si>
+  <si>
+    <t>Hammer Punch</t>
+  </si>
+  <si>
+    <t>Soco de Martelo</t>
+  </si>
+  <si>
+    <t>Servant Protection</t>
+  </si>
+  <si>
+    <t>Proteção de Servos</t>
+  </si>
+  <si>
+    <t>Take out Garbage</t>
+  </si>
+  <si>
+    <t>Tirar a Sujeira</t>
+  </si>
+  <si>
+    <t>Dark Revival</t>
+  </si>
+  <si>
+    <t>Reanimação Obscura</t>
+  </si>
+  <si>
+    <t>Skull Initialization</t>
+  </si>
+  <si>
+    <t>Inicialização de Crânio</t>
+  </si>
+  <si>
+    <t>Percepção de Crânio</t>
+  </si>
+  <si>
+    <t>Notice Skull</t>
+  </si>
+  <si>
+    <t>Aparição de Crânio</t>
+  </si>
+  <si>
+    <t>Skull Appears</t>
+  </si>
+  <si>
+    <t>Whirlwind Demon</t>
+  </si>
+  <si>
+    <t>Demônio do Redemoinho</t>
+  </si>
+  <si>
+    <t>Throw Knife</t>
+  </si>
+  <si>
+    <t>Atirar Faca</t>
+  </si>
+  <si>
+    <t>Dispelling Punch</t>
+  </si>
+  <si>
+    <t>Soco Dissipador</t>
+  </si>
+  <si>
+    <t>Spinning Slash</t>
+  </si>
+  <si>
+    <t>Corte Giratório</t>
+  </si>
+  <si>
+    <t>Gatling Knife</t>
+  </si>
+  <si>
+    <t>Metralhadora de Facas</t>
+  </si>
+  <si>
+    <t>Chop Up</t>
+  </si>
+  <si>
+    <t>Esquartejar</t>
+  </si>
+  <si>
+    <t>Tormenta de Facas</t>
+  </si>
+  <si>
+    <t>Knife Storm</t>
+  </si>
+  <si>
+    <t>Raging Flames</t>
+  </si>
+  <si>
+    <t>Chamas Furiosas</t>
+  </si>
+  <si>
+    <t>Rolling Punch</t>
+  </si>
+  <si>
+    <t>Soco de Rolo</t>
+  </si>
+  <si>
+    <t>Superheated Breath</t>
+  </si>
+  <si>
+    <t>Bafo Superaquecido</t>
+  </si>
+  <si>
+    <t>Multi-Shot</t>
+  </si>
+  <si>
+    <t>Múltiplos Disparos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flash Bang </t>
+  </si>
+  <si>
+    <t>Explosão Luminosa</t>
+  </si>
+  <si>
+    <t>Quick Draw</t>
+  </si>
+  <si>
+    <t>Saque Rápido</t>
+  </si>
+  <si>
+    <t>Gunman Mode</t>
+  </si>
+  <si>
+    <t>Modo Pistoleiro</t>
+  </si>
+  <si>
+    <t>Charged Shot</t>
+  </si>
+  <si>
+    <t>Disparo Carregado</t>
+  </si>
+  <si>
+    <t>Bystander</t>
+  </si>
+  <si>
+    <t>Transeunte</t>
+  </si>
+  <si>
+    <t>Kingly Mode</t>
+  </si>
+  <si>
+    <t>Modo Majestoso</t>
+  </si>
+  <si>
+    <t>Earth Shock</t>
+  </si>
+  <si>
+    <t>Choque de Terra</t>
+  </si>
+  <si>
+    <t>Smack Down</t>
+  </si>
+  <si>
+    <t>Abater</t>
+  </si>
+  <si>
+    <t>Glare</t>
+  </si>
+  <si>
+    <t>Replendor</t>
+  </si>
+  <si>
+    <t>Ice Claw</t>
+  </si>
+  <si>
+    <t>Garra de Gelo</t>
+  </si>
+  <si>
+    <t>Wolf Preemptive Strike</t>
+  </si>
+  <si>
+    <t>Ataque Preventivo de Lobo</t>
+  </si>
+  <si>
+    <t>Tail Defense</t>
+  </si>
+  <si>
+    <t>Defesa de Cauda</t>
+  </si>
+  <si>
+    <t>Trample</t>
+  </si>
+  <si>
+    <t>Pisotear</t>
+  </si>
+  <si>
+    <t>Habilidades</t>
   </si>
 </sst>
 </file>
@@ -1495,7 +1740,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1506,7 +1751,7 @@
   <dimension ref="B1:E42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:C18"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2063,8 +2308,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G68"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2611,10 +2856,10 @@
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
+        <v>364</v>
+      </c>
+      <c r="C68" t="s">
         <v>365</v>
-      </c>
-      <c r="C68" t="s">
-        <v>366</v>
       </c>
     </row>
   </sheetData>
@@ -2631,10 +2876,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:C63"/>
+  <dimension ref="B1:C104"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C63"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2645,16 +2890,16 @@
   <sheetData>
     <row r="1" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
-        <v>315</v>
+        <v>458</v>
       </c>
       <c r="C1" s="3"/>
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C2" t="s">
         <v>359</v>
-      </c>
-      <c r="C2" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
@@ -2667,492 +2912,821 @@
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>361</v>
+        <v>394</v>
       </c>
       <c r="C4" t="s">
-        <v>362</v>
+        <v>395</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>296</v>
+        <v>360</v>
       </c>
       <c r="C5" t="s">
-        <v>297</v>
+        <v>361</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>254</v>
+        <v>390</v>
       </c>
       <c r="C6" t="s">
-        <v>255</v>
+        <v>391</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>345</v>
+        <v>296</v>
       </c>
       <c r="C7" t="s">
-        <v>346</v>
+        <v>297</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>310</v>
+        <v>254</v>
       </c>
       <c r="C8" t="s">
-        <v>311</v>
+        <v>255</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>250</v>
+        <v>440</v>
       </c>
       <c r="C9" t="s">
-        <v>251</v>
+        <v>441</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>282</v>
+        <v>344</v>
       </c>
       <c r="C10" t="s">
-        <v>283</v>
+        <v>345</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>244</v>
+        <v>438</v>
       </c>
       <c r="C11" t="s">
-        <v>245</v>
+        <v>439</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>276</v>
+        <v>420</v>
       </c>
       <c r="C12" t="s">
-        <v>277</v>
+        <v>421</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>280</v>
+        <v>310</v>
       </c>
       <c r="C13" t="s">
-        <v>281</v>
+        <v>311</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>326</v>
+        <v>250</v>
       </c>
       <c r="C14" t="s">
-        <v>327</v>
+        <v>251</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>290</v>
+        <v>402</v>
       </c>
       <c r="C15" t="s">
-        <v>291</v>
+        <v>403</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>252</v>
+        <v>282</v>
       </c>
       <c r="C16" t="s">
-        <v>253</v>
+        <v>283</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>367</v>
+        <v>388</v>
       </c>
       <c r="C17" t="s">
-        <v>368</v>
+        <v>389</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>288</v>
+        <v>414</v>
       </c>
       <c r="C18" t="s">
-        <v>289</v>
+        <v>415</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>256</v>
+        <v>244</v>
       </c>
       <c r="C19" t="s">
-        <v>257</v>
+        <v>245</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>351</v>
+        <v>244</v>
       </c>
       <c r="C20" t="s">
-        <v>352</v>
+        <v>245</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="C21" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>341</v>
+        <v>378</v>
       </c>
       <c r="C22" t="s">
-        <v>342</v>
+        <v>379</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>294</v>
+        <v>280</v>
       </c>
       <c r="C23" t="s">
-        <v>295</v>
+        <v>281</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>375</v>
+        <v>444</v>
       </c>
       <c r="C24" t="s">
-        <v>376</v>
+        <v>445</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>363</v>
+        <v>325</v>
       </c>
       <c r="C25" t="s">
-        <v>364</v>
+        <v>326</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>304</v>
+        <v>290</v>
       </c>
       <c r="C26" t="s">
-        <v>305</v>
+        <v>291</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>347</v>
+        <v>252</v>
       </c>
       <c r="C27" t="s">
-        <v>348</v>
+        <v>253</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>264</v>
+        <v>366</v>
       </c>
       <c r="C28" t="s">
-        <v>265</v>
+        <v>367</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>266</v>
+        <v>288</v>
       </c>
       <c r="C29" t="s">
-        <v>267</v>
+        <v>289</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>333</v>
+        <v>256</v>
       </c>
       <c r="C30" t="s">
-        <v>334</v>
+        <v>257</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>292</v>
+        <v>350</v>
       </c>
       <c r="C31" t="s">
-        <v>293</v>
+        <v>351</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>302</v>
+        <v>432</v>
       </c>
       <c r="C32" t="s">
-        <v>303</v>
+        <v>433</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>300</v>
+        <v>272</v>
       </c>
       <c r="C33" t="s">
-        <v>301</v>
+        <v>273</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>262</v>
+        <v>340</v>
       </c>
       <c r="C34" t="s">
-        <v>263</v>
+        <v>341</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>373</v>
+        <v>418</v>
       </c>
       <c r="C35" t="s">
-        <v>374</v>
+        <v>419</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>339</v>
+        <v>448</v>
       </c>
       <c r="C36" t="s">
-        <v>340</v>
+        <v>449</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>258</v>
+        <v>294</v>
       </c>
       <c r="C37" t="s">
-        <v>259</v>
+        <v>295</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>298</v>
+        <v>436</v>
       </c>
       <c r="C38" t="s">
-        <v>299</v>
+        <v>437</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>357</v>
+        <v>396</v>
       </c>
       <c r="C39" t="s">
-        <v>358</v>
+        <v>397</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>335</v>
+        <v>374</v>
       </c>
       <c r="C40" t="s">
-        <v>336</v>
+        <v>375</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>284</v>
+        <v>362</v>
       </c>
       <c r="C41" t="s">
-        <v>285</v>
+        <v>363</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>355</v>
+        <v>304</v>
       </c>
       <c r="C42" t="s">
-        <v>356</v>
+        <v>305</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="C43" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>270</v>
+        <v>450</v>
       </c>
       <c r="C44" t="s">
-        <v>271</v>
+        <v>451</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>312</v>
+        <v>384</v>
       </c>
       <c r="C45" t="s">
-        <v>313</v>
+        <v>385</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>313</v>
+        <v>442</v>
       </c>
       <c r="C46" t="s">
-        <v>314</v>
+        <v>443</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>248</v>
+        <v>423</v>
       </c>
       <c r="C47" t="s">
-        <v>249</v>
+        <v>422</v>
       </c>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>337</v>
+        <v>382</v>
       </c>
       <c r="C48" t="s">
-        <v>338</v>
+        <v>383</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>308</v>
+        <v>264</v>
       </c>
       <c r="C49" t="s">
-        <v>309</v>
+        <v>265</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>353</v>
+        <v>266</v>
       </c>
       <c r="C50" t="s">
-        <v>354</v>
+        <v>267</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>324</v>
+        <v>332</v>
       </c>
       <c r="C51" t="s">
-        <v>325</v>
+        <v>333</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>268</v>
+        <v>292</v>
       </c>
       <c r="C52" t="s">
-        <v>269</v>
+        <v>293</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>322</v>
+        <v>302</v>
       </c>
       <c r="C53" t="s">
-        <v>323</v>
+        <v>303</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>377</v>
+        <v>300</v>
       </c>
       <c r="C54" t="s">
-        <v>378</v>
+        <v>301</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>286</v>
+        <v>262</v>
       </c>
       <c r="C55" t="s">
-        <v>287</v>
+        <v>263</v>
       </c>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>260</v>
+        <v>372</v>
       </c>
       <c r="C56" t="s">
-        <v>261</v>
+        <v>373</v>
       </c>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="C57" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>246</v>
+        <v>258</v>
       </c>
       <c r="C58" t="s">
-        <v>247</v>
+        <v>259</v>
       </c>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="C59" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>369</v>
+        <v>356</v>
       </c>
       <c r="C60" t="s">
-        <v>370</v>
+        <v>357</v>
       </c>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>371</v>
+        <v>334</v>
       </c>
       <c r="C61" t="s">
-        <v>372</v>
+        <v>335</v>
       </c>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>320</v>
+        <v>430</v>
       </c>
       <c r="C62" t="s">
-        <v>321</v>
+        <v>431</v>
       </c>
     </row>
     <row r="63" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
+        <v>386</v>
+      </c>
+      <c r="C63" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>407</v>
+      </c>
+      <c r="C64" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>284</v>
+      </c>
+      <c r="C65" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>354</v>
+      </c>
+      <c r="C66" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>348</v>
+      </c>
+      <c r="C67" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>380</v>
+      </c>
+      <c r="C68" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>270</v>
+      </c>
+      <c r="C69" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>312</v>
+      </c>
+      <c r="C70" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>313</v>
+      </c>
+      <c r="C71" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>248</v>
+      </c>
+      <c r="C72" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="73" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
+        <v>434</v>
+      </c>
+      <c r="C73" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="74" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
+        <v>424</v>
+      </c>
+      <c r="C74" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="75" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
+        <v>336</v>
+      </c>
+      <c r="C75" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="76" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
+        <v>308</v>
+      </c>
+      <c r="C76" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="77" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
+        <v>426</v>
+      </c>
+      <c r="C77" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="78" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
+        <v>398</v>
+      </c>
+      <c r="C78" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="79" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B79" t="s">
+        <v>352</v>
+      </c>
+      <c r="C79" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="80" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
+        <v>323</v>
+      </c>
+      <c r="C80" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
+        <v>409</v>
+      </c>
+      <c r="C81" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="82" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
+        <v>404</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
+        <v>446</v>
+      </c>
+      <c r="C83" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="84" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
+        <v>268</v>
+      </c>
+      <c r="C84" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="85" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
+        <v>321</v>
+      </c>
+      <c r="C85" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
+        <v>416</v>
+      </c>
+      <c r="C86" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="87" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
+        <v>393</v>
+      </c>
+      <c r="C87" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="88" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B88" t="s">
+        <v>376</v>
+      </c>
+      <c r="C88" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="89" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
+        <v>286</v>
+      </c>
+      <c r="C89" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="90" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B90" t="s">
+        <v>260</v>
+      </c>
+      <c r="C90" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="91" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B91" t="s">
+        <v>428</v>
+      </c>
+      <c r="C91" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="92" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B92" t="s">
+        <v>342</v>
+      </c>
+      <c r="C92" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="93" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B93" t="s">
+        <v>246</v>
+      </c>
+      <c r="C93" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="94" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B94" t="s">
+        <v>306</v>
+      </c>
+      <c r="C94" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="95" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B95" t="s">
+        <v>454</v>
+      </c>
+      <c r="C95" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="96" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B96" t="s">
+        <v>368</v>
+      </c>
+      <c r="C96" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="97" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B97" t="s">
+        <v>400</v>
+      </c>
+      <c r="C97" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B98" t="s">
+        <v>412</v>
+      </c>
+      <c r="C98" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B99" t="s">
+        <v>456</v>
+      </c>
+      <c r="C99" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B100" t="s">
+        <v>370</v>
+      </c>
+      <c r="C100" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="101" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B101" t="s">
+        <v>319</v>
+      </c>
+      <c r="C101" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="102" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B102" t="s">
+        <v>410</v>
+      </c>
+      <c r="C102" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="103" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B103" t="s">
         <v>278</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C103" t="s">
         <v>279</v>
       </c>
     </row>
+    <row r="104" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B104" t="s">
+        <v>452</v>
+      </c>
+      <c r="C104" t="s">
+        <v>453</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="B2:C63">
+  <sortState ref="B2:C104">
     <sortCondition ref="B2"/>
   </sortState>
   <mergeCells count="1">
     <mergeCell ref="B1:C1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3172,24 +3746,24 @@
   <sheetData>
     <row r="1" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C1" s="3"/>
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
+        <v>316</v>
+      </c>
+      <c r="C2" t="s">
         <v>317</v>
-      </c>
-      <c r="C2" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
@@ -3202,18 +3776,18 @@
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
+        <v>327</v>
+      </c>
+      <c r="C5" t="s">
         <v>328</v>
-      </c>
-      <c r="C5" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
+        <v>329</v>
+      </c>
+      <c r="C6" t="s">
         <v>330</v>
-      </c>
-      <c r="C6" t="s">
-        <v>331</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
revisão mes_wd01_01_us.u16 e mes_wd01_01_us.u16 e atualização do glossario.xlsx
</commit_message>
<xml_diff>
--- a/glossario.xlsx
+++ b/glossario.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Diversos" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="497">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="503">
   <si>
     <t>Aerial Troop</t>
   </si>
@@ -1520,6 +1520,24 @@
   </si>
   <si>
     <t>Atque Pisoteio</t>
+  </si>
+  <si>
+    <t>Valley of Murals</t>
+  </si>
+  <si>
+    <t>Vale dos Murais</t>
+  </si>
+  <si>
+    <t>Mechat Dock</t>
+  </si>
+  <si>
+    <t>Doca do Mecóptero</t>
+  </si>
+  <si>
+    <t>Upper Mecha Base</t>
+  </si>
+  <si>
+    <t>Base Mecanoide Superior</t>
   </si>
 </sst>
 </file>
@@ -2195,10 +2213,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D25"/>
+  <dimension ref="B1:D28"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2404,6 +2422,30 @@
       </c>
       <c r="C25" t="s">
         <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>497</v>
+      </c>
+      <c r="C26" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>499</v>
+      </c>
+      <c r="C27" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>501</v>
+      </c>
+      <c r="C28" t="s">
+        <v>502</v>
       </c>
     </row>
   </sheetData>
@@ -2992,7 +3034,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+    <sheetView topLeftCell="A93" workbookViewId="0">
       <selection activeCell="C114" sqref="C114"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Traduzido SkWd_new_us.u16 até linha 1.400. Atualizado glossario.xlsx~
</commit_message>
<xml_diff>
--- a/glossario.xlsx
+++ b/glossario.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moacyr\Desktop\GITHUB-BLUE DRAGON\traducao-blue-dragon-xbox360\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\danger\traducoes\traducao-blue-dragon-xbox360\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Diversos" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="503">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="561">
   <si>
     <t>Aerial Troop</t>
   </si>
@@ -1519,9 +1519,6 @@
     <t>Stomp Attack</t>
   </si>
   <si>
-    <t>Atque Pisoteio</t>
-  </si>
-  <si>
     <t>Valley of Murals</t>
   </si>
   <si>
@@ -1538,6 +1535,183 @@
   </si>
   <si>
     <t>Base Mecanoide Superior</t>
+  </si>
+  <si>
+    <t>Ataque Pisoteio</t>
+  </si>
+  <si>
+    <t>Cheerful Sound</t>
+  </si>
+  <si>
+    <t>Som Alegre</t>
+  </si>
+  <si>
+    <t>Clobber</t>
+  </si>
+  <si>
+    <t>Espancar</t>
+  </si>
+  <si>
+    <t>Quick Dry</t>
+  </si>
+  <si>
+    <t>Secagem Rápida</t>
+  </si>
+  <si>
+    <t>Mist Step</t>
+  </si>
+  <si>
+    <t>Passo de Névoa</t>
+  </si>
+  <si>
+    <t>Tail Whip</t>
+  </si>
+  <si>
+    <t>Chicote de Cauda</t>
+  </si>
+  <si>
+    <t>Black Wind</t>
+  </si>
+  <si>
+    <t>Vento Negro</t>
+  </si>
+  <si>
+    <t>Blow Away</t>
+  </si>
+  <si>
+    <t>Sopro</t>
+  </si>
+  <si>
+    <t>Multiple Stab</t>
+  </si>
+  <si>
+    <t>Facada Múltipla</t>
+  </si>
+  <si>
+    <t>Lighten</t>
+  </si>
+  <si>
+    <t>Aliviar</t>
+  </si>
+  <si>
+    <t>Critical Breakthrough</t>
+  </si>
+  <si>
+    <t>Avanço Crítico</t>
+  </si>
+  <si>
+    <t>Throw Staff</t>
+  </si>
+  <si>
+    <t>Lançar Cajado</t>
+  </si>
+  <si>
+    <t>Drill Attack</t>
+  </si>
+  <si>
+    <t>Ataque Perfurante</t>
+  </si>
+  <si>
+    <t>Skewer</t>
+  </si>
+  <si>
+    <t>Espeto</t>
+  </si>
+  <si>
+    <t>Raging Multi-Strike</t>
+  </si>
+  <si>
+    <t>Multi-Ataque Furioso</t>
+  </si>
+  <si>
+    <t>Rattling Tail</t>
+  </si>
+  <si>
+    <t>Cauda de Cascavel</t>
+  </si>
+  <si>
+    <t>Claw of Evil Warding</t>
+  </si>
+  <si>
+    <t>Garra de Proteção do Mal</t>
+  </si>
+  <si>
+    <t>Body Slam</t>
+  </si>
+  <si>
+    <t>Golpe Corporal</t>
+  </si>
+  <si>
+    <t>Multi-Strike</t>
+  </si>
+  <si>
+    <t>Multi-Ataque</t>
+  </si>
+  <si>
+    <t>Wallop</t>
+  </si>
+  <si>
+    <t>Porrada</t>
+  </si>
+  <si>
+    <t>Mirror Coating</t>
+  </si>
+  <si>
+    <t>Revestimento Espelhado</t>
+  </si>
+  <si>
+    <t>Raging Slash</t>
+  </si>
+  <si>
+    <t>Corte Furioso</t>
+  </si>
+  <si>
+    <t>Burn Down</t>
+  </si>
+  <si>
+    <t>Calcinação</t>
+  </si>
+  <si>
+    <t>Become Hyper</t>
+  </si>
+  <si>
+    <t>Nervosismo</t>
+  </si>
+  <si>
+    <t>Hyper Trigger</t>
+  </si>
+  <si>
+    <t>Desencadeador de Nervos</t>
+  </si>
+  <si>
+    <t>Spiteful Dance</t>
+  </si>
+  <si>
+    <t>Dança Destrutiva</t>
+  </si>
+  <si>
+    <t>Vanishing Dance</t>
+  </si>
+  <si>
+    <t>Dança Efêmera</t>
+  </si>
+  <si>
+    <t>Scatter Money</t>
+  </si>
+  <si>
+    <t>Trocado</t>
+  </si>
+  <si>
+    <t>Demonic Lullaby</t>
+  </si>
+  <si>
+    <t>Canção de Ninar Demoníaca</t>
+  </si>
+  <si>
+    <t>Ice Grind</t>
+  </si>
+  <si>
+    <t>Moagem de Gelo</t>
   </si>
 </sst>
 </file>
@@ -2215,7 +2389,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
@@ -2426,26 +2600,26 @@
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
+        <v>496</v>
+      </c>
+      <c r="C26" t="s">
         <v>497</v>
-      </c>
-      <c r="C26" t="s">
-        <v>498</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
+        <v>498</v>
+      </c>
+      <c r="C27" t="s">
         <v>499</v>
-      </c>
-      <c r="C27" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
+        <v>500</v>
+      </c>
+      <c r="C28" t="s">
         <v>501</v>
-      </c>
-      <c r="C28" t="s">
-        <v>502</v>
       </c>
     </row>
   </sheetData>
@@ -2464,8 +2638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G68"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2892,134 +3066,134 @@
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>176</v>
+        <v>364</v>
       </c>
       <c r="C53" t="s">
-        <v>179</v>
+        <v>365</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C54" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C55" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>158</v>
+        <v>178</v>
       </c>
       <c r="C56" t="s">
-        <v>161</v>
+        <v>181</v>
       </c>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C57" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C58" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>103</v>
+        <v>160</v>
       </c>
       <c r="C59" t="s">
-        <v>106</v>
+        <v>163</v>
       </c>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C60" t="s">
-        <v>124</v>
+        <v>106</v>
       </c>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C61" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C62" t="s">
-        <v>110</v>
+        <v>125</v>
       </c>
     </row>
     <row r="63" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C63" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C64" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>231</v>
+        <v>109</v>
       </c>
       <c r="C65" t="s">
-        <v>233</v>
+        <v>123</v>
       </c>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C66" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C67" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>364</v>
+        <v>230</v>
       </c>
       <c r="C68" t="s">
-        <v>365</v>
+        <v>235</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="B2:C67">
+  <sortState ref="B2:C68">
     <sortCondition ref="B2"/>
   </sortState>
   <mergeCells count="1">
@@ -3032,10 +3206,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:C114"/>
+  <dimension ref="B1:C143"/>
   <sheetViews>
-    <sheetView topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="C114" sqref="C114"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:C143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3068,894 +3242,1126 @@
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>394</v>
+        <v>547</v>
       </c>
       <c r="C4" t="s">
-        <v>395</v>
+        <v>548</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>360</v>
+        <v>513</v>
       </c>
       <c r="C5" t="s">
-        <v>361</v>
+        <v>514</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
       <c r="C6" t="s">
-        <v>391</v>
+        <v>395</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>296</v>
+        <v>360</v>
       </c>
       <c r="C7" t="s">
-        <v>297</v>
+        <v>361</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>254</v>
+        <v>390</v>
       </c>
       <c r="C8" t="s">
-        <v>255</v>
+        <v>391</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>440</v>
+        <v>515</v>
       </c>
       <c r="C9" t="s">
-        <v>441</v>
+        <v>516</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>344</v>
-      </c>
-      <c r="C10" t="s">
-        <v>345</v>
+        <v>535</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>536</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>438</v>
+        <v>296</v>
       </c>
       <c r="C11" t="s">
-        <v>439</v>
+        <v>297</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>420</v>
+        <v>254</v>
       </c>
       <c r="C12" t="s">
-        <v>421</v>
+        <v>255</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>310</v>
+        <v>545</v>
       </c>
       <c r="C13" t="s">
-        <v>311</v>
+        <v>546</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>250</v>
+        <v>440</v>
       </c>
       <c r="C14" t="s">
-        <v>251</v>
+        <v>441</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>402</v>
+        <v>344</v>
       </c>
       <c r="C15" t="s">
-        <v>403</v>
+        <v>345</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>282</v>
+        <v>438</v>
       </c>
       <c r="C16" t="s">
-        <v>283</v>
+        <v>439</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>388</v>
+        <v>503</v>
       </c>
       <c r="C17" t="s">
-        <v>389</v>
+        <v>504</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>414</v>
+        <v>420</v>
       </c>
       <c r="C18" t="s">
-        <v>415</v>
+        <v>421</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>244</v>
-      </c>
-      <c r="C19" t="s">
-        <v>245</v>
+        <v>533</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>534</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>244</v>
+        <v>505</v>
       </c>
       <c r="C20" t="s">
-        <v>245</v>
+        <v>506</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>276</v>
+        <v>310</v>
       </c>
       <c r="C21" t="s">
-        <v>277</v>
+        <v>311</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>378</v>
+        <v>250</v>
       </c>
       <c r="C22" t="s">
-        <v>379</v>
+        <v>251</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>280</v>
+        <v>521</v>
       </c>
       <c r="C23" t="s">
-        <v>281</v>
+        <v>522</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>444</v>
+        <v>402</v>
       </c>
       <c r="C24" t="s">
-        <v>445</v>
+        <v>403</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>325</v>
+        <v>282</v>
       </c>
       <c r="C25" t="s">
-        <v>326</v>
+        <v>283</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>290</v>
+        <v>557</v>
       </c>
       <c r="C26" t="s">
-        <v>291</v>
+        <v>558</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>252</v>
+        <v>388</v>
       </c>
       <c r="C27" t="s">
-        <v>253</v>
+        <v>389</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>366</v>
+        <v>414</v>
       </c>
       <c r="C28" t="s">
-        <v>367</v>
+        <v>415</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>288</v>
+        <v>244</v>
       </c>
       <c r="C29" t="s">
-        <v>289</v>
+        <v>245</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>256</v>
+        <v>244</v>
       </c>
       <c r="C30" t="s">
-        <v>257</v>
+        <v>245</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>350</v>
+        <v>276</v>
       </c>
       <c r="C31" t="s">
-        <v>351</v>
+        <v>277</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>432</v>
-      </c>
-      <c r="C32" t="s">
-        <v>433</v>
+        <v>525</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>526</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>272</v>
+        <v>378</v>
       </c>
       <c r="C33" t="s">
-        <v>273</v>
+        <v>379</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>340</v>
+        <v>280</v>
       </c>
       <c r="C34" t="s">
-        <v>341</v>
+        <v>281</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>418</v>
+        <v>444</v>
       </c>
       <c r="C35" t="s">
-        <v>419</v>
+        <v>445</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>448</v>
+        <v>325</v>
       </c>
       <c r="C36" t="s">
-        <v>449</v>
+        <v>326</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="C37" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>436</v>
+        <v>252</v>
       </c>
       <c r="C38" t="s">
-        <v>437</v>
+        <v>253</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>396</v>
+        <v>366</v>
       </c>
       <c r="C39" t="s">
-        <v>397</v>
+        <v>367</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>374</v>
+        <v>288</v>
       </c>
       <c r="C40" t="s">
-        <v>375</v>
+        <v>289</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>362</v>
+        <v>256</v>
       </c>
       <c r="C41" t="s">
-        <v>363</v>
+        <v>257</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>304</v>
+        <v>350</v>
       </c>
       <c r="C42" t="s">
-        <v>305</v>
+        <v>351</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>346</v>
+        <v>432</v>
       </c>
       <c r="C43" t="s">
-        <v>347</v>
+        <v>433</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>450</v>
+        <v>272</v>
       </c>
       <c r="C44" t="s">
-        <v>451</v>
+        <v>273</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>384</v>
+        <v>340</v>
       </c>
       <c r="C45" t="s">
-        <v>385</v>
+        <v>341</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>442</v>
+        <v>418</v>
       </c>
       <c r="C46" t="s">
-        <v>443</v>
+        <v>419</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>423</v>
+        <v>480</v>
       </c>
       <c r="C47" t="s">
-        <v>422</v>
+        <v>481</v>
       </c>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>382</v>
+        <v>448</v>
       </c>
       <c r="C48" t="s">
-        <v>383</v>
+        <v>449</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>264</v>
+        <v>294</v>
       </c>
       <c r="C49" t="s">
-        <v>265</v>
+        <v>295</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>266</v>
+        <v>436</v>
       </c>
       <c r="C50" t="s">
-        <v>267</v>
+        <v>437</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>332</v>
+        <v>396</v>
       </c>
       <c r="C51" t="s">
-        <v>333</v>
+        <v>397</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>292</v>
+        <v>374</v>
       </c>
       <c r="C52" t="s">
-        <v>293</v>
+        <v>375</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>302</v>
+        <v>362</v>
       </c>
       <c r="C53" t="s">
-        <v>303</v>
+        <v>363</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="C54" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>262</v>
+        <v>549</v>
       </c>
       <c r="C55" t="s">
-        <v>263</v>
+        <v>550</v>
       </c>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>372</v>
+        <v>346</v>
       </c>
       <c r="C56" t="s">
-        <v>373</v>
+        <v>347</v>
       </c>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>338</v>
+        <v>450</v>
       </c>
       <c r="C57" t="s">
-        <v>339</v>
+        <v>451</v>
       </c>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>258</v>
+        <v>559</v>
       </c>
       <c r="C58" t="s">
-        <v>259</v>
+        <v>560</v>
       </c>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>298</v>
+        <v>384</v>
       </c>
       <c r="C59" t="s">
-        <v>299</v>
+        <v>385</v>
       </c>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>356</v>
+        <v>442</v>
       </c>
       <c r="C60" t="s">
-        <v>357</v>
+        <v>443</v>
       </c>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>334</v>
+        <v>423</v>
       </c>
       <c r="C61" t="s">
-        <v>335</v>
+        <v>422</v>
       </c>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>430</v>
+        <v>382</v>
       </c>
       <c r="C62" t="s">
-        <v>431</v>
+        <v>383</v>
       </c>
     </row>
     <row r="63" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>386</v>
+        <v>264</v>
       </c>
       <c r="C63" t="s">
-        <v>387</v>
+        <v>265</v>
       </c>
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>407</v>
+        <v>266</v>
       </c>
       <c r="C64" t="s">
-        <v>406</v>
+        <v>267</v>
       </c>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>284</v>
+        <v>519</v>
       </c>
       <c r="C65" t="s">
-        <v>285</v>
+        <v>520</v>
       </c>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>354</v>
+        <v>483</v>
       </c>
       <c r="C66" t="s">
-        <v>355</v>
+        <v>484</v>
       </c>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>348</v>
+        <v>332</v>
       </c>
       <c r="C67" t="s">
-        <v>349</v>
+        <v>333</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>380</v>
+        <v>292</v>
       </c>
       <c r="C68" t="s">
-        <v>381</v>
+        <v>293</v>
       </c>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>270</v>
+        <v>302</v>
       </c>
       <c r="C69" t="s">
-        <v>271</v>
+        <v>303</v>
       </c>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>312</v>
+        <v>300</v>
       </c>
       <c r="C70" t="s">
-        <v>313</v>
+        <v>301</v>
       </c>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>313</v>
+        <v>262</v>
       </c>
       <c r="C71" t="s">
-        <v>314</v>
+        <v>263</v>
       </c>
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>248</v>
+        <v>372</v>
       </c>
       <c r="C72" t="s">
-        <v>249</v>
+        <v>373</v>
       </c>
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>434</v>
+        <v>338</v>
       </c>
       <c r="C73" t="s">
-        <v>435</v>
+        <v>339</v>
       </c>
     </row>
     <row r="74" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>424</v>
+        <v>541</v>
       </c>
       <c r="C74" t="s">
-        <v>425</v>
+        <v>542</v>
       </c>
     </row>
     <row r="75" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>336</v>
+        <v>258</v>
       </c>
       <c r="C75" t="s">
-        <v>337</v>
+        <v>259</v>
       </c>
     </row>
     <row r="76" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>308</v>
+        <v>298</v>
       </c>
       <c r="C76" t="s">
-        <v>309</v>
+        <v>299</v>
       </c>
     </row>
     <row r="77" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>426</v>
+        <v>509</v>
       </c>
       <c r="C77" t="s">
-        <v>427</v>
+        <v>510</v>
       </c>
     </row>
     <row r="78" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>398</v>
+        <v>475</v>
       </c>
       <c r="C78" t="s">
-        <v>399</v>
+        <v>476</v>
       </c>
     </row>
     <row r="79" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>352</v>
+        <v>356</v>
       </c>
       <c r="C79" t="s">
-        <v>353</v>
+        <v>357</v>
       </c>
     </row>
     <row r="80" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>323</v>
+        <v>334</v>
       </c>
       <c r="C80" t="s">
-        <v>324</v>
+        <v>335</v>
       </c>
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>409</v>
+        <v>517</v>
       </c>
       <c r="C81" t="s">
-        <v>408</v>
+        <v>518</v>
       </c>
     </row>
     <row r="82" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>404</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>405</v>
+        <v>430</v>
+      </c>
+      <c r="C82" t="s">
+        <v>431</v>
       </c>
     </row>
     <row r="83" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>446</v>
+        <v>537</v>
       </c>
       <c r="C83" t="s">
-        <v>447</v>
+        <v>538</v>
       </c>
     </row>
     <row r="84" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>268</v>
+        <v>386</v>
       </c>
       <c r="C84" t="s">
-        <v>269</v>
+        <v>387</v>
       </c>
     </row>
     <row r="85" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>321</v>
+        <v>407</v>
       </c>
       <c r="C85" t="s">
-        <v>322</v>
+        <v>406</v>
       </c>
     </row>
     <row r="86" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>416</v>
+        <v>284</v>
       </c>
       <c r="C86" t="s">
-        <v>417</v>
+        <v>285</v>
       </c>
     </row>
     <row r="87" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>393</v>
+        <v>354</v>
       </c>
       <c r="C87" t="s">
-        <v>392</v>
+        <v>355</v>
       </c>
     </row>
     <row r="88" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
-        <v>376</v>
+        <v>348</v>
       </c>
       <c r="C88" t="s">
-        <v>377</v>
+        <v>349</v>
       </c>
     </row>
     <row r="89" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
-        <v>286</v>
+        <v>380</v>
       </c>
       <c r="C89" t="s">
-        <v>287</v>
+        <v>381</v>
       </c>
     </row>
     <row r="90" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
-        <v>260</v>
+        <v>485</v>
       </c>
       <c r="C90" t="s">
-        <v>261</v>
+        <v>486</v>
       </c>
     </row>
     <row r="91" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
-        <v>428</v>
+        <v>270</v>
       </c>
       <c r="C91" t="s">
-        <v>429</v>
+        <v>271</v>
       </c>
     </row>
     <row r="92" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
-        <v>342</v>
+        <v>312</v>
       </c>
       <c r="C92" t="s">
-        <v>343</v>
+        <v>313</v>
       </c>
     </row>
     <row r="93" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
-        <v>246</v>
+        <v>313</v>
       </c>
       <c r="C93" t="s">
-        <v>247</v>
+        <v>314</v>
       </c>
     </row>
     <row r="94" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
-        <v>306</v>
+        <v>248</v>
       </c>
       <c r="C94" t="s">
-        <v>307</v>
+        <v>249</v>
       </c>
     </row>
     <row r="95" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
-        <v>454</v>
+        <v>434</v>
       </c>
       <c r="C95" t="s">
-        <v>455</v>
+        <v>435</v>
       </c>
     </row>
     <row r="96" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
-        <v>368</v>
+        <v>507</v>
       </c>
       <c r="C96" t="s">
-        <v>369</v>
+        <v>508</v>
       </c>
     </row>
     <row r="97" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
-        <v>400</v>
+        <v>424</v>
       </c>
       <c r="C97" t="s">
-        <v>401</v>
+        <v>425</v>
       </c>
     </row>
     <row r="98" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
-        <v>412</v>
-      </c>
-      <c r="C98" t="s">
-        <v>413</v>
+        <v>529</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>530</v>
       </c>
     </row>
     <row r="99" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
-        <v>456</v>
+        <v>543</v>
       </c>
       <c r="C99" t="s">
-        <v>457</v>
+        <v>544</v>
       </c>
     </row>
     <row r="100" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
-        <v>370</v>
+        <v>336</v>
       </c>
       <c r="C100" t="s">
-        <v>371</v>
+        <v>337</v>
       </c>
     </row>
     <row r="101" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
-        <v>319</v>
-      </c>
-      <c r="C101" t="s">
-        <v>320</v>
+        <v>531</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>532</v>
       </c>
     </row>
     <row r="102" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
-        <v>410</v>
+        <v>308</v>
       </c>
       <c r="C102" t="s">
-        <v>411</v>
+        <v>309</v>
       </c>
     </row>
     <row r="103" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
-        <v>278</v>
+        <v>477</v>
       </c>
       <c r="C103" t="s">
-        <v>279</v>
+        <v>478</v>
       </c>
     </row>
     <row r="104" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
-        <v>452</v>
+        <v>484</v>
       </c>
       <c r="C104" t="s">
-        <v>453</v>
+        <v>485</v>
       </c>
     </row>
     <row r="105" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
-        <v>471</v>
+        <v>426</v>
       </c>
       <c r="C105" t="s">
-        <v>472</v>
+        <v>427</v>
       </c>
     </row>
     <row r="106" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
-        <v>474</v>
+        <v>555</v>
       </c>
       <c r="C106" t="s">
-        <v>473</v>
+        <v>556</v>
       </c>
     </row>
     <row r="107" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
-        <v>475</v>
+        <v>398</v>
       </c>
       <c r="C107" t="s">
-        <v>476</v>
+        <v>399</v>
       </c>
     </row>
     <row r="108" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
-        <v>477</v>
+        <v>352</v>
       </c>
       <c r="C108" t="s">
-        <v>478</v>
+        <v>353</v>
       </c>
     </row>
     <row r="109" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
-        <v>479</v>
+        <v>323</v>
       </c>
       <c r="C109" t="s">
-        <v>482</v>
+        <v>324</v>
       </c>
     </row>
     <row r="110" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
-        <v>480</v>
-      </c>
-      <c r="C110" t="s">
-        <v>481</v>
+        <v>527</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>528</v>
       </c>
     </row>
     <row r="111" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
-        <v>483</v>
+        <v>409</v>
       </c>
       <c r="C111" t="s">
-        <v>484</v>
+        <v>408</v>
       </c>
     </row>
     <row r="112" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
-        <v>484</v>
-      </c>
-      <c r="C112" t="s">
-        <v>485</v>
+        <v>404</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="113" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
-        <v>485</v>
+        <v>446</v>
       </c>
       <c r="C113" t="s">
-        <v>486</v>
+        <v>447</v>
       </c>
     </row>
     <row r="114" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
+        <v>268</v>
+      </c>
+      <c r="C114" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="115" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B115" t="s">
+        <v>321</v>
+      </c>
+      <c r="C115" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="116" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B116" t="s">
+        <v>416</v>
+      </c>
+      <c r="C116" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="117" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B117" t="s">
+        <v>551</v>
+      </c>
+      <c r="C117" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="118" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B118" t="s">
+        <v>393</v>
+      </c>
+      <c r="C118" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="119" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B119" t="s">
+        <v>376</v>
+      </c>
+      <c r="C119" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="120" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B120" t="s">
         <v>495</v>
       </c>
-      <c r="C114" t="s">
-        <v>496</v>
+      <c r="C120" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="121" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B121" t="s">
+        <v>286</v>
+      </c>
+      <c r="C121" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="122" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B122" t="s">
+        <v>260</v>
+      </c>
+      <c r="C122" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="123" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B123" t="s">
+        <v>471</v>
+      </c>
+      <c r="C123" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="124" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B124" t="s">
+        <v>428</v>
+      </c>
+      <c r="C124" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="125" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B125" t="s">
+        <v>474</v>
+      </c>
+      <c r="C125" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="126" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B126" t="s">
+        <v>342</v>
+      </c>
+      <c r="C126" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="127" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B127" t="s">
+        <v>246</v>
+      </c>
+      <c r="C127" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="128" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B128" t="s">
+        <v>306</v>
+      </c>
+      <c r="C128" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="129" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B129" t="s">
+        <v>454</v>
+      </c>
+      <c r="C129" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="130" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B130" t="s">
+        <v>368</v>
+      </c>
+      <c r="C130" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="131" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B131" t="s">
+        <v>511</v>
+      </c>
+      <c r="C131" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="132" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B132" t="s">
+        <v>400</v>
+      </c>
+      <c r="C132" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="133" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B133" t="s">
+        <v>479</v>
+      </c>
+      <c r="C133" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="134" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B134" t="s">
+        <v>412</v>
+      </c>
+      <c r="C134" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="135" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B135" t="s">
+        <v>523</v>
+      </c>
+      <c r="C135" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="136" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B136" t="s">
+        <v>456</v>
+      </c>
+      <c r="C136" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="137" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B137" t="s">
+        <v>370</v>
+      </c>
+      <c r="C137" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="138" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B138" t="s">
+        <v>553</v>
+      </c>
+      <c r="C138" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="139" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B139" t="s">
+        <v>539</v>
+      </c>
+      <c r="C139" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="140" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B140" t="s">
+        <v>319</v>
+      </c>
+      <c r="C140" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="141" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B141" t="s">
+        <v>410</v>
+      </c>
+      <c r="C141" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="142" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B142" t="s">
+        <v>278</v>
+      </c>
+      <c r="C142" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="143" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B143" t="s">
+        <v>452</v>
+      </c>
+      <c r="C143" t="s">
+        <v>453</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="B2:C104">
+  <sortState ref="B2:C143">
     <sortCondition ref="B2"/>
   </sortState>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Traduzidas primeiras linhas do ItWd_us.u16
</commit_message>
<xml_diff>
--- a/glossario.xlsx
+++ b/glossario.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moacyr\Desktop\GITHUB-BLUE DRAGON\traducao-blue-dragon-xbox360\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\danger\traducoes\traducao-blue-dragon-xbox360\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Diversos" sheetId="2" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Magias" sheetId="3" r:id="rId4"/>
     <sheet name="Habilidades" sheetId="7" r:id="rId5"/>
     <sheet name="Monstros" sheetId="8" r:id="rId6"/>
+    <sheet name="Itens" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="144525"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="581">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="590">
   <si>
     <t>Aerial Troop</t>
   </si>
@@ -1772,6 +1773,33 @@
   </si>
   <si>
     <t>Picanço Basilisco</t>
+  </si>
+  <si>
+    <t>Medicine</t>
+  </si>
+  <si>
+    <t>Itens</t>
+  </si>
+  <si>
+    <t>Medicamento</t>
+  </si>
+  <si>
+    <t>Dungeon</t>
+  </si>
+  <si>
+    <t>Masmorra</t>
+  </si>
+  <si>
+    <t>Elixir</t>
+  </si>
+  <si>
+    <t>Radiant Flour</t>
+  </si>
+  <si>
+    <t>Head Doctor</t>
+  </si>
+  <si>
+    <t>Médico-Chefe</t>
   </si>
 </sst>
 </file>
@@ -2117,7 +2145,7 @@
   <dimension ref="B1:E42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2142,118 +2170,130 @@
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>4</v>
+        <v>242</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>243</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" t="s">
-        <v>18</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="E8" s="1"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>14</v>
+        <v>588</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>589</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>13</v>
+      </c>
+      <c r="D13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="C14" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>242</v>
+        <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>243</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="42" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D42" s="1"/>
     </row>
   </sheetData>
+  <sortState ref="B2:C16">
+    <sortCondition ref="B2"/>
+  </sortState>
   <mergeCells count="1">
     <mergeCell ref="B1:C1"/>
   </mergeCells>
@@ -2449,7 +2489,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D28"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
@@ -2696,10 +2736,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G74"/>
+  <dimension ref="B1:G75"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3299,6 +3339,11 @@
       </c>
       <c r="C74" t="s">
         <v>235</v>
+      </c>
+    </row>
+    <row r="75" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
+        <v>587</v>
       </c>
     </row>
   </sheetData>
@@ -4493,8 +4538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4662,4 +4707,56 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.5703125" customWidth="1"/>
+    <col min="3" max="3" width="31.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
+        <v>582</v>
+      </c>
+      <c r="C1" s="3"/>
+    </row>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>581</v>
+      </c>
+      <c r="C2" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>584</v>
+      </c>
+      <c r="C3" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>586</v>
+      </c>
+      <c r="C4" t="s">
+        <v>586</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Traduzido até linha 300 do arquivo com as colunas 0 e 3.
</commit_message>
<xml_diff>
--- a/glossario.xlsx
+++ b/glossario.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moacyr\Desktop\GITHUB-BLUE DRAGON\traducao-blue-dragon-xbox360\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\danger\traducoes\traducao-blue-dragon-xbox360\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Diversos" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="591">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="652">
   <si>
     <t>Aerial Troop</t>
   </si>
@@ -629,9 +629,6 @@
     <t>Deflect</t>
   </si>
   <si>
-    <t>Acurácia</t>
-  </si>
-  <si>
     <t>Curse</t>
   </si>
   <si>
@@ -1803,6 +1800,192 @@
   </si>
   <si>
     <t>Blizzard Dragon</t>
+  </si>
+  <si>
+    <t>Flawless Amethyst</t>
+  </si>
+  <si>
+    <t>Ametista Perfeita</t>
+  </si>
+  <si>
+    <t>Poison Powder</t>
+  </si>
+  <si>
+    <t>Pó Venenoso</t>
+  </si>
+  <si>
+    <t>Sleep Powder</t>
+  </si>
+  <si>
+    <t>Sonífero</t>
+  </si>
+  <si>
+    <t>Stink</t>
+  </si>
+  <si>
+    <t>Fedor</t>
+  </si>
+  <si>
+    <t>Mobility Balm</t>
+  </si>
+  <si>
+    <t>Bálsamo de Mobilidade</t>
+  </si>
+  <si>
+    <t>No-Ghost Device</t>
+  </si>
+  <si>
+    <t>Mecanismo Sem-Fantasma</t>
+  </si>
+  <si>
+    <t>Mirror Earring</t>
+  </si>
+  <si>
+    <t>Brinco Espelhado</t>
+  </si>
+  <si>
+    <t>Alacrity Elixir</t>
+  </si>
+  <si>
+    <t>Elixir de Presteza</t>
+  </si>
+  <si>
+    <t>Iridescent Cyclone</t>
+  </si>
+  <si>
+    <t>Ciclone Iridescente</t>
+  </si>
+  <si>
+    <t>Ancient Phonograph</t>
+  </si>
+  <si>
+    <t>Gramofone Ancestral</t>
+  </si>
+  <si>
+    <t>Thorn Grass</t>
+  </si>
+  <si>
+    <t>Thorn Vines</t>
+  </si>
+  <si>
+    <t>Thorn Branch</t>
+  </si>
+  <si>
+    <t>Videira de Espinhos</t>
+  </si>
+  <si>
+    <t>Relva de Espinhos</t>
+  </si>
+  <si>
+    <t>Ramo de Espinhos</t>
+  </si>
+  <si>
+    <t>Steadiness Salve</t>
+  </si>
+  <si>
+    <t>Bálsamo da Estabilidade</t>
+  </si>
+  <si>
+    <t>Power-Swap Dart</t>
+  </si>
+  <si>
+    <t>Dardo Permutador</t>
+  </si>
+  <si>
+    <t>MP Boost Elixir</t>
+  </si>
+  <si>
+    <t>Elixir Potencializador de MP</t>
+  </si>
+  <si>
+    <t>Repeater Weed</t>
+  </si>
+  <si>
+    <t>Erva de Réplica</t>
+  </si>
+  <si>
+    <t>Stout Garlic</t>
+  </si>
+  <si>
+    <t>Alho Forte</t>
+  </si>
+  <si>
+    <t>Farinha Radiante</t>
+  </si>
+  <si>
+    <t>Zephyr Chocolate</t>
+  </si>
+  <si>
+    <t>Chocolate da Vitalidade</t>
+  </si>
+  <si>
+    <t>Ancient Feather</t>
+  </si>
+  <si>
+    <t>Pluma Ancestral</t>
+  </si>
+  <si>
+    <t>Shell Badge</t>
+  </si>
+  <si>
+    <t>Placa de Carapaça</t>
+  </si>
+  <si>
+    <t>Shield Badge</t>
+  </si>
+  <si>
+    <t>Placa de Escudo</t>
+  </si>
+  <si>
+    <t>Moody Dragon's Fang</t>
+  </si>
+  <si>
+    <t>Presa do Dragão Mal-Humorado</t>
+  </si>
+  <si>
+    <t>Phantom Dragon's Fang</t>
+  </si>
+  <si>
+    <t>Presa do Dragão Espectral</t>
+  </si>
+  <si>
+    <t>Bellybutton Ring of Earth</t>
+  </si>
+  <si>
+    <t>Piercing de Terra</t>
+  </si>
+  <si>
+    <t>Crown of the King Ghost</t>
+  </si>
+  <si>
+    <t>Coroa do Rei Espectral</t>
+  </si>
+  <si>
+    <t>HP Up Elixir</t>
+  </si>
+  <si>
+    <t>Elixir de HP Superior</t>
+  </si>
+  <si>
+    <t>Body Builder's Elixir</t>
+  </si>
+  <si>
+    <t>Elixir do Fisiculturista</t>
+  </si>
+  <si>
+    <t>Evasiva</t>
+  </si>
+  <si>
+    <t>HP Max Up</t>
+  </si>
+  <si>
+    <t>Max HP +</t>
+  </si>
+  <si>
+    <t>Magic Atk Up</t>
+  </si>
+  <si>
+    <t>Ataque Mágico +</t>
   </si>
 </sst>
 </file>
@@ -2181,10 +2364,10 @@
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>241</v>
+      </c>
+      <c r="C4" t="s">
         <v>242</v>
-      </c>
-      <c r="C4" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
@@ -2222,10 +2405,10 @@
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
+        <v>587</v>
+      </c>
+      <c r="C9" t="s">
         <v>588</v>
-      </c>
-      <c r="C9" t="s">
-        <v>589</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
@@ -2493,7 +2676,7 @@
   <dimension ref="B1:D28"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2703,26 +2886,26 @@
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
+        <v>494</v>
+      </c>
+      <c r="C26" t="s">
         <v>495</v>
-      </c>
-      <c r="C26" t="s">
-        <v>496</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
+        <v>496</v>
+      </c>
+      <c r="C27" t="s">
         <v>497</v>
-      </c>
-      <c r="C27" t="s">
-        <v>498</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
+        <v>498</v>
+      </c>
+      <c r="C28" t="s">
         <v>499</v>
-      </c>
-      <c r="C28" t="s">
-        <v>500</v>
       </c>
     </row>
   </sheetData>
@@ -2739,10 +2922,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G75"/>
+  <dimension ref="B1:G77"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="B75" sqref="B75"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2759,18 +2942,18 @@
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
+        <v>220</v>
+      </c>
+      <c r="C2" t="s">
         <v>221</v>
-      </c>
-      <c r="C2" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C3" t="s">
         <v>200</v>
-      </c>
-      <c r="C3" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
@@ -2786,7 +2969,7 @@
         <v>198</v>
       </c>
       <c r="C5" t="s">
-        <v>199</v>
+        <v>647</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
@@ -2807,26 +2990,26 @@
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C9" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
@@ -2879,478 +3062,498 @@
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C17" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C18" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C19" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>94</v>
+        <v>648</v>
       </c>
       <c r="C20" t="s">
-        <v>95</v>
+        <v>649</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>562</v>
+        <v>94</v>
       </c>
       <c r="C21" t="s">
-        <v>563</v>
+        <v>95</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>566</v>
+        <v>650</v>
       </c>
       <c r="C22" t="s">
-        <v>564</v>
+        <v>651</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="C23" t="s">
-        <v>573</v>
+        <v>562</v>
       </c>
       <c r="G23" s="2"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>170</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>171</v>
+        <v>565</v>
+      </c>
+      <c r="C24" t="s">
+        <v>563</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>87</v>
+        <v>564</v>
       </c>
       <c r="C25" t="s">
-        <v>88</v>
+        <v>572</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>93</v>
+      <c r="B27" t="s">
+        <v>87</v>
+      </c>
+      <c r="C27" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>228</v>
-      </c>
-      <c r="C28" t="s">
-        <v>229</v>
+        <v>172</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>202</v>
-      </c>
-      <c r="C29" t="s">
-        <v>205</v>
+      <c r="B29" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>203</v>
+        <v>227</v>
       </c>
       <c r="C30" t="s">
-        <v>206</v>
+        <v>228</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
+        <v>201</v>
+      </c>
+      <c r="C31" t="s">
         <v>204</v>
-      </c>
-      <c r="C31" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>182</v>
+        <v>202</v>
       </c>
       <c r="C32" t="s">
-        <v>184</v>
+        <v>205</v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>183</v>
+        <v>203</v>
       </c>
       <c r="C33" t="s">
-        <v>185</v>
+        <v>206</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>226</v>
+        <v>182</v>
       </c>
       <c r="C34" t="s">
-        <v>225</v>
+        <v>184</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>223</v>
+        <v>183</v>
       </c>
       <c r="C35" t="s">
-        <v>224</v>
+        <v>185</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>567</v>
+        <v>225</v>
       </c>
       <c r="C36" t="s">
-        <v>568</v>
+        <v>224</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>569</v>
+        <v>222</v>
       </c>
       <c r="C37" t="s">
-        <v>570</v>
+        <v>223</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>571</v>
+        <v>566</v>
       </c>
       <c r="C38" t="s">
-        <v>572</v>
+        <v>567</v>
       </c>
       <c r="F38" s="1"/>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>164</v>
+        <v>568</v>
       </c>
       <c r="C39" t="s">
-        <v>168</v>
+        <v>569</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>165</v>
+        <v>570</v>
       </c>
       <c r="C40" t="s">
-        <v>169</v>
+        <v>571</v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C41" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>227</v>
+        <v>165</v>
       </c>
       <c r="C42" t="s">
-        <v>227</v>
+        <v>169</v>
       </c>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="C43" t="s">
-        <v>99</v>
+        <v>174</v>
       </c>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>97</v>
+        <v>226</v>
       </c>
       <c r="C44" t="s">
-        <v>118</v>
+        <v>226</v>
       </c>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C45" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>186</v>
+        <v>97</v>
       </c>
       <c r="C46" t="s">
-        <v>190</v>
+        <v>118</v>
       </c>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>187</v>
+        <v>98</v>
       </c>
       <c r="C47" t="s">
-        <v>189</v>
+        <v>121</v>
       </c>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
+        <v>186</v>
+      </c>
+      <c r="C48" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>187</v>
+      </c>
+      <c r="C49" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
         <v>188</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C50" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
+    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
         <v>192</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="C51" s="2" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
+    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
         <v>193</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="C52" s="2" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
+    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
         <v>194</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C53" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
+    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
         <v>100</v>
       </c>
-      <c r="C52" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
+      <c r="C54" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
         <v>101</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C55" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
+    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
         <v>175</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C56" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
+    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>207</v>
+      </c>
+      <c r="C57" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
         <v>208</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C58" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B56" t="s">
+    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
         <v>209</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C59" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
-        <v>210</v>
-      </c>
-      <c r="C57" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B58" t="s">
+    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
         <v>89</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C60" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B59" t="s">
+    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>596</v>
+      </c>
+      <c r="C61" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>362</v>
+      </c>
+      <c r="C62" t="s">
         <v>363</v>
       </c>
-      <c r="C59" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B60" t="s">
+    </row>
+    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
         <v>176</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C63" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B61" t="s">
+    <row r="64" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
         <v>177</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C64" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B62" t="s">
-        <v>178</v>
-      </c>
-      <c r="C62" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B63" t="s">
-        <v>158</v>
-      </c>
-      <c r="C63" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B64" t="s">
-        <v>159</v>
-      </c>
-      <c r="C64" t="s">
-        <v>162</v>
-      </c>
+      <c r="F64" s="1"/>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>160</v>
+        <v>178</v>
       </c>
       <c r="C65" t="s">
-        <v>163</v>
+        <v>181</v>
       </c>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>103</v>
+        <v>158</v>
       </c>
       <c r="C66" t="s">
-        <v>106</v>
+        <v>161</v>
       </c>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>104</v>
+        <v>159</v>
       </c>
       <c r="C67" t="s">
-        <v>124</v>
+        <v>162</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>105</v>
+        <v>160</v>
       </c>
       <c r="C68" t="s">
-        <v>125</v>
+        <v>163</v>
       </c>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C69" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C70" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C71" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>231</v>
+        <v>107</v>
       </c>
       <c r="C72" t="s">
-        <v>233</v>
+        <v>110</v>
       </c>
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>232</v>
+        <v>108</v>
       </c>
       <c r="C73" t="s">
-        <v>234</v>
+        <v>122</v>
       </c>
     </row>
     <row r="74" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>230</v>
+        <v>109</v>
       </c>
       <c r="C74" t="s">
-        <v>235</v>
+        <v>123</v>
       </c>
     </row>
     <row r="75" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>587</v>
+        <v>230</v>
+      </c>
+      <c r="C75" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="76" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
+        <v>231</v>
+      </c>
+      <c r="C76" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="77" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
+        <v>229</v>
+      </c>
+      <c r="C77" t="s">
+        <v>234</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="B2:C74">
+  <sortState ref="B2:C77">
     <sortCondition ref="B2"/>
   </sortState>
   <mergeCells count="1">
@@ -3377,1152 +3580,1152 @@
   <sheetData>
     <row r="1" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C1" s="3"/>
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
+        <v>356</v>
+      </c>
+      <c r="C2" t="s">
         <v>357</v>
-      </c>
-      <c r="C2" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
+        <v>310</v>
+      </c>
+      <c r="C3" t="s">
         <v>311</v>
-      </c>
-      <c r="C3" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>545</v>
+      </c>
+      <c r="C4" t="s">
         <v>546</v>
-      </c>
-      <c r="C4" t="s">
-        <v>547</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
+        <v>511</v>
+      </c>
+      <c r="C5" t="s">
         <v>512</v>
-      </c>
-      <c r="C5" t="s">
-        <v>513</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
+        <v>392</v>
+      </c>
+      <c r="C6" t="s">
         <v>393</v>
-      </c>
-      <c r="C6" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
+        <v>358</v>
+      </c>
+      <c r="C7" t="s">
         <v>359</v>
-      </c>
-      <c r="C7" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
+        <v>388</v>
+      </c>
+      <c r="C8" t="s">
         <v>389</v>
-      </c>
-      <c r="C8" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
+        <v>513</v>
+      </c>
+      <c r="C9" t="s">
         <v>514</v>
-      </c>
-      <c r="C9" t="s">
-        <v>515</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
+        <v>533</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>534</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>535</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
+        <v>295</v>
+      </c>
+      <c r="C11" t="s">
         <v>296</v>
-      </c>
-      <c r="C11" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
+        <v>253</v>
+      </c>
+      <c r="C12" t="s">
         <v>254</v>
-      </c>
-      <c r="C12" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
+        <v>543</v>
+      </c>
+      <c r="C13" t="s">
         <v>544</v>
-      </c>
-      <c r="C13" t="s">
-        <v>545</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
+        <v>438</v>
+      </c>
+      <c r="C14" t="s">
         <v>439</v>
-      </c>
-      <c r="C14" t="s">
-        <v>440</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
+        <v>342</v>
+      </c>
+      <c r="C15" t="s">
         <v>343</v>
-      </c>
-      <c r="C15" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
+        <v>436</v>
+      </c>
+      <c r="C16" t="s">
         <v>437</v>
-      </c>
-      <c r="C16" t="s">
-        <v>438</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
+        <v>501</v>
+      </c>
+      <c r="C17" t="s">
         <v>502</v>
-      </c>
-      <c r="C17" t="s">
-        <v>503</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
+        <v>418</v>
+      </c>
+      <c r="C18" t="s">
         <v>419</v>
-      </c>
-      <c r="C18" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
+        <v>531</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>532</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>533</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
+        <v>503</v>
+      </c>
+      <c r="C20" t="s">
         <v>504</v>
-      </c>
-      <c r="C20" t="s">
-        <v>505</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
+        <v>309</v>
+      </c>
+      <c r="C21" t="s">
         <v>310</v>
-      </c>
-      <c r="C21" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
+        <v>249</v>
+      </c>
+      <c r="C22" t="s">
         <v>250</v>
-      </c>
-      <c r="C22" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
+        <v>519</v>
+      </c>
+      <c r="C23" t="s">
         <v>520</v>
-      </c>
-      <c r="C23" t="s">
-        <v>521</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
+        <v>400</v>
+      </c>
+      <c r="C24" t="s">
         <v>401</v>
-      </c>
-      <c r="C24" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
+        <v>281</v>
+      </c>
+      <c r="C25" t="s">
         <v>282</v>
-      </c>
-      <c r="C25" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
+        <v>555</v>
+      </c>
+      <c r="C26" t="s">
         <v>556</v>
-      </c>
-      <c r="C26" t="s">
-        <v>557</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
+        <v>386</v>
+      </c>
+      <c r="C27" t="s">
         <v>387</v>
-      </c>
-      <c r="C27" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
+        <v>412</v>
+      </c>
+      <c r="C28" t="s">
         <v>413</v>
-      </c>
-      <c r="C28" t="s">
-        <v>414</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
+        <v>243</v>
+      </c>
+      <c r="C29" t="s">
         <v>244</v>
-      </c>
-      <c r="C29" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
+        <v>243</v>
+      </c>
+      <c r="C30" t="s">
         <v>244</v>
-      </c>
-      <c r="C30" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
+        <v>275</v>
+      </c>
+      <c r="C31" t="s">
         <v>276</v>
-      </c>
-      <c r="C31" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
+        <v>523</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>524</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>525</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
+        <v>376</v>
+      </c>
+      <c r="C33" t="s">
         <v>377</v>
-      </c>
-      <c r="C33" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
+        <v>279</v>
+      </c>
+      <c r="C34" t="s">
         <v>280</v>
-      </c>
-      <c r="C34" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
+        <v>442</v>
+      </c>
+      <c r="C35" t="s">
         <v>443</v>
-      </c>
-      <c r="C35" t="s">
-        <v>444</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
+        <v>323</v>
+      </c>
+      <c r="C36" t="s">
         <v>324</v>
-      </c>
-      <c r="C36" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
+        <v>289</v>
+      </c>
+      <c r="C37" t="s">
         <v>290</v>
-      </c>
-      <c r="C37" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
+        <v>251</v>
+      </c>
+      <c r="C38" t="s">
         <v>252</v>
-      </c>
-      <c r="C38" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
+        <v>364</v>
+      </c>
+      <c r="C39" t="s">
         <v>365</v>
-      </c>
-      <c r="C39" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
+        <v>287</v>
+      </c>
+      <c r="C40" t="s">
         <v>288</v>
-      </c>
-      <c r="C40" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
+        <v>255</v>
+      </c>
+      <c r="C41" t="s">
         <v>256</v>
-      </c>
-      <c r="C41" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
+        <v>348</v>
+      </c>
+      <c r="C42" t="s">
         <v>349</v>
-      </c>
-      <c r="C42" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
+        <v>430</v>
+      </c>
+      <c r="C43" t="s">
         <v>431</v>
-      </c>
-      <c r="C43" t="s">
-        <v>432</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
+        <v>271</v>
+      </c>
+      <c r="C44" t="s">
         <v>272</v>
-      </c>
-      <c r="C44" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
+        <v>338</v>
+      </c>
+      <c r="C45" t="s">
         <v>339</v>
-      </c>
-      <c r="C45" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
+        <v>416</v>
+      </c>
+      <c r="C46" t="s">
         <v>417</v>
-      </c>
-      <c r="C46" t="s">
-        <v>418</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
+        <v>478</v>
+      </c>
+      <c r="C47" t="s">
         <v>479</v>
-      </c>
-      <c r="C47" t="s">
-        <v>480</v>
       </c>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
+        <v>446</v>
+      </c>
+      <c r="C48" t="s">
         <v>447</v>
-      </c>
-      <c r="C48" t="s">
-        <v>448</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
+        <v>293</v>
+      </c>
+      <c r="C49" t="s">
         <v>294</v>
-      </c>
-      <c r="C49" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
+        <v>434</v>
+      </c>
+      <c r="C50" t="s">
         <v>435</v>
-      </c>
-      <c r="C50" t="s">
-        <v>436</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
+        <v>394</v>
+      </c>
+      <c r="C51" t="s">
         <v>395</v>
-      </c>
-      <c r="C51" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
+        <v>372</v>
+      </c>
+      <c r="C52" t="s">
         <v>373</v>
-      </c>
-      <c r="C52" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
+        <v>559</v>
+      </c>
+      <c r="C53" t="s">
         <v>560</v>
-      </c>
-      <c r="C53" t="s">
-        <v>561</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
+        <v>360</v>
+      </c>
+      <c r="C54" t="s">
         <v>361</v>
-      </c>
-      <c r="C54" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
+        <v>303</v>
+      </c>
+      <c r="C55" t="s">
         <v>304</v>
-      </c>
-      <c r="C55" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
+        <v>547</v>
+      </c>
+      <c r="C56" t="s">
         <v>548</v>
-      </c>
-      <c r="C56" t="s">
-        <v>549</v>
       </c>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
+        <v>344</v>
+      </c>
+      <c r="C57" t="s">
         <v>345</v>
-      </c>
-      <c r="C57" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
+        <v>448</v>
+      </c>
+      <c r="C58" t="s">
         <v>449</v>
-      </c>
-      <c r="C58" t="s">
-        <v>450</v>
       </c>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
+        <v>557</v>
+      </c>
+      <c r="C59" t="s">
         <v>558</v>
-      </c>
-      <c r="C59" t="s">
-        <v>559</v>
       </c>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
+        <v>382</v>
+      </c>
+      <c r="C60" t="s">
         <v>383</v>
-      </c>
-      <c r="C60" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
+        <v>440</v>
+      </c>
+      <c r="C61" t="s">
         <v>441</v>
-      </c>
-      <c r="C61" t="s">
-        <v>442</v>
       </c>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C62" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="63" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
+        <v>380</v>
+      </c>
+      <c r="C63" t="s">
         <v>381</v>
-      </c>
-      <c r="C63" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
+        <v>263</v>
+      </c>
+      <c r="C64" t="s">
         <v>264</v>
-      </c>
-      <c r="C64" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
+        <v>265</v>
+      </c>
+      <c r="C65" t="s">
         <v>266</v>
-      </c>
-      <c r="C65" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
+        <v>517</v>
+      </c>
+      <c r="C66" t="s">
         <v>518</v>
-      </c>
-      <c r="C66" t="s">
-        <v>519</v>
       </c>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
+        <v>481</v>
+      </c>
+      <c r="C67" t="s">
         <v>482</v>
-      </c>
-      <c r="C67" t="s">
-        <v>483</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
+        <v>330</v>
+      </c>
+      <c r="C68" t="s">
         <v>331</v>
-      </c>
-      <c r="C68" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
+        <v>291</v>
+      </c>
+      <c r="C69" t="s">
         <v>292</v>
-      </c>
-      <c r="C69" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
+        <v>301</v>
+      </c>
+      <c r="C70" t="s">
         <v>302</v>
-      </c>
-      <c r="C70" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
+        <v>299</v>
+      </c>
+      <c r="C71" t="s">
         <v>300</v>
-      </c>
-      <c r="C71" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
+        <v>261</v>
+      </c>
+      <c r="C72" t="s">
         <v>262</v>
-      </c>
-      <c r="C72" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
+        <v>370</v>
+      </c>
+      <c r="C73" t="s">
         <v>371</v>
-      </c>
-      <c r="C73" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="74" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
+        <v>336</v>
+      </c>
+      <c r="C74" t="s">
         <v>337</v>
-      </c>
-      <c r="C74" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="75" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
+        <v>539</v>
+      </c>
+      <c r="C75" t="s">
         <v>540</v>
-      </c>
-      <c r="C75" t="s">
-        <v>541</v>
       </c>
     </row>
     <row r="76" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
+        <v>257</v>
+      </c>
+      <c r="C76" t="s">
         <v>258</v>
-      </c>
-      <c r="C76" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="77" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
+        <v>297</v>
+      </c>
+      <c r="C77" t="s">
         <v>298</v>
-      </c>
-      <c r="C77" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="78" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
+        <v>507</v>
+      </c>
+      <c r="C78" t="s">
         <v>508</v>
-      </c>
-      <c r="C78" t="s">
-        <v>509</v>
       </c>
     </row>
     <row r="79" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
+        <v>473</v>
+      </c>
+      <c r="C79" t="s">
         <v>474</v>
-      </c>
-      <c r="C79" t="s">
-        <v>475</v>
       </c>
     </row>
     <row r="80" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
+        <v>354</v>
+      </c>
+      <c r="C80" t="s">
         <v>355</v>
-      </c>
-      <c r="C80" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
+        <v>332</v>
+      </c>
+      <c r="C81" t="s">
         <v>333</v>
-      </c>
-      <c r="C81" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="82" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
+        <v>515</v>
+      </c>
+      <c r="C82" t="s">
         <v>516</v>
-      </c>
-      <c r="C82" t="s">
-        <v>517</v>
       </c>
     </row>
     <row r="83" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
+        <v>428</v>
+      </c>
+      <c r="C83" t="s">
         <v>429</v>
-      </c>
-      <c r="C83" t="s">
-        <v>430</v>
       </c>
     </row>
     <row r="84" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
+        <v>535</v>
+      </c>
+      <c r="C84" t="s">
         <v>536</v>
-      </c>
-      <c r="C84" t="s">
-        <v>537</v>
       </c>
     </row>
     <row r="85" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
+        <v>384</v>
+      </c>
+      <c r="C85" t="s">
         <v>385</v>
-      </c>
-      <c r="C85" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="86" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C86" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="87" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
+        <v>283</v>
+      </c>
+      <c r="C87" t="s">
         <v>284</v>
-      </c>
-      <c r="C87" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="88" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
+        <v>352</v>
+      </c>
+      <c r="C88" t="s">
         <v>353</v>
-      </c>
-      <c r="C88" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="89" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
+        <v>346</v>
+      </c>
+      <c r="C89" t="s">
         <v>347</v>
-      </c>
-      <c r="C89" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="90" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
+        <v>378</v>
+      </c>
+      <c r="C90" t="s">
         <v>379</v>
-      </c>
-      <c r="C90" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="91" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
+        <v>483</v>
+      </c>
+      <c r="C91" t="s">
         <v>484</v>
-      </c>
-      <c r="C91" t="s">
-        <v>485</v>
       </c>
     </row>
     <row r="92" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
+        <v>269</v>
+      </c>
+      <c r="C92" t="s">
         <v>270</v>
-      </c>
-      <c r="C92" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="93" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
+        <v>311</v>
+      </c>
+      <c r="C93" t="s">
         <v>312</v>
-      </c>
-      <c r="C93" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="94" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
+        <v>312</v>
+      </c>
+      <c r="C94" t="s">
         <v>313</v>
-      </c>
-      <c r="C94" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="95" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
+        <v>247</v>
+      </c>
+      <c r="C95" t="s">
         <v>248</v>
-      </c>
-      <c r="C95" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="96" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
+        <v>432</v>
+      </c>
+      <c r="C96" t="s">
         <v>433</v>
-      </c>
-      <c r="C96" t="s">
-        <v>434</v>
       </c>
     </row>
     <row r="97" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
+        <v>505</v>
+      </c>
+      <c r="C97" t="s">
         <v>506</v>
-      </c>
-      <c r="C97" t="s">
-        <v>507</v>
       </c>
     </row>
     <row r="98" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
+        <v>422</v>
+      </c>
+      <c r="C98" t="s">
         <v>423</v>
-      </c>
-      <c r="C98" t="s">
-        <v>424</v>
       </c>
     </row>
     <row r="99" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
+        <v>527</v>
+      </c>
+      <c r="C99" s="2" t="s">
         <v>528</v>
-      </c>
-      <c r="C99" s="2" t="s">
-        <v>529</v>
       </c>
     </row>
     <row r="100" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
+        <v>541</v>
+      </c>
+      <c r="C100" t="s">
         <v>542</v>
-      </c>
-      <c r="C100" t="s">
-        <v>543</v>
       </c>
     </row>
     <row r="101" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
+        <v>334</v>
+      </c>
+      <c r="C101" t="s">
         <v>335</v>
-      </c>
-      <c r="C101" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="102" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
+        <v>529</v>
+      </c>
+      <c r="C102" s="2" t="s">
         <v>530</v>
-      </c>
-      <c r="C102" s="2" t="s">
-        <v>531</v>
       </c>
     </row>
     <row r="103" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
+        <v>307</v>
+      </c>
+      <c r="C103" t="s">
         <v>308</v>
-      </c>
-      <c r="C103" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="104" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
+        <v>475</v>
+      </c>
+      <c r="C104" t="s">
         <v>476</v>
-      </c>
-      <c r="C104" t="s">
-        <v>477</v>
       </c>
     </row>
     <row r="105" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
+        <v>482</v>
+      </c>
+      <c r="C105" t="s">
         <v>483</v>
-      </c>
-      <c r="C105" t="s">
-        <v>484</v>
       </c>
     </row>
     <row r="106" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
+        <v>424</v>
+      </c>
+      <c r="C106" t="s">
         <v>425</v>
-      </c>
-      <c r="C106" t="s">
-        <v>426</v>
       </c>
     </row>
     <row r="107" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
+        <v>553</v>
+      </c>
+      <c r="C107" t="s">
         <v>554</v>
-      </c>
-      <c r="C107" t="s">
-        <v>555</v>
       </c>
     </row>
     <row r="108" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
+        <v>396</v>
+      </c>
+      <c r="C108" t="s">
         <v>397</v>
-      </c>
-      <c r="C108" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="109" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
+        <v>350</v>
+      </c>
+      <c r="C109" t="s">
         <v>351</v>
-      </c>
-      <c r="C109" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="110" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
+        <v>321</v>
+      </c>
+      <c r="C110" t="s">
         <v>322</v>
-      </c>
-      <c r="C110" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="111" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
+        <v>525</v>
+      </c>
+      <c r="C111" s="2" t="s">
         <v>526</v>
-      </c>
-      <c r="C111" s="2" t="s">
-        <v>527</v>
       </c>
     </row>
     <row r="112" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C112" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="113" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
+        <v>402</v>
+      </c>
+      <c r="C113" s="2" t="s">
         <v>403</v>
-      </c>
-      <c r="C113" s="2" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="114" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
+        <v>444</v>
+      </c>
+      <c r="C114" t="s">
         <v>445</v>
-      </c>
-      <c r="C114" t="s">
-        <v>446</v>
       </c>
     </row>
     <row r="115" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
+        <v>267</v>
+      </c>
+      <c r="C115" t="s">
         <v>268</v>
-      </c>
-      <c r="C115" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="116" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
+        <v>319</v>
+      </c>
+      <c r="C116" t="s">
         <v>320</v>
-      </c>
-      <c r="C116" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="117" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
+        <v>414</v>
+      </c>
+      <c r="C117" t="s">
         <v>415</v>
-      </c>
-      <c r="C117" t="s">
-        <v>416</v>
       </c>
     </row>
     <row r="118" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
+        <v>549</v>
+      </c>
+      <c r="C118" t="s">
         <v>550</v>
-      </c>
-      <c r="C118" t="s">
-        <v>551</v>
       </c>
     </row>
     <row r="119" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C119" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="120" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
+        <v>374</v>
+      </c>
+      <c r="C120" t="s">
         <v>375</v>
-      </c>
-      <c r="C120" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="121" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C121" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="122" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
+        <v>285</v>
+      </c>
+      <c r="C122" t="s">
         <v>286</v>
-      </c>
-      <c r="C122" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="123" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
+        <v>259</v>
+      </c>
+      <c r="C123" t="s">
         <v>260</v>
-      </c>
-      <c r="C123" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="124" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
+        <v>469</v>
+      </c>
+      <c r="C124" t="s">
         <v>470</v>
-      </c>
-      <c r="C124" t="s">
-        <v>471</v>
       </c>
     </row>
     <row r="125" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
+        <v>426</v>
+      </c>
+      <c r="C125" t="s">
         <v>427</v>
-      </c>
-      <c r="C125" t="s">
-        <v>428</v>
       </c>
     </row>
     <row r="126" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C126" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="127" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
+        <v>340</v>
+      </c>
+      <c r="C127" t="s">
         <v>341</v>
-      </c>
-      <c r="C127" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="128" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
+        <v>245</v>
+      </c>
+      <c r="C128" t="s">
         <v>246</v>
-      </c>
-      <c r="C128" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="129" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
+        <v>305</v>
+      </c>
+      <c r="C129" t="s">
         <v>306</v>
-      </c>
-      <c r="C129" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="130" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B130" t="s">
+        <v>452</v>
+      </c>
+      <c r="C130" t="s">
         <v>453</v>
-      </c>
-      <c r="C130" t="s">
-        <v>454</v>
       </c>
     </row>
     <row r="131" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
+        <v>366</v>
+      </c>
+      <c r="C131" t="s">
         <v>367</v>
-      </c>
-      <c r="C131" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="132" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
+        <v>509</v>
+      </c>
+      <c r="C132" t="s">
         <v>510</v>
-      </c>
-      <c r="C132" t="s">
-        <v>511</v>
       </c>
     </row>
     <row r="133" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B133" t="s">
+        <v>398</v>
+      </c>
+      <c r="C133" t="s">
         <v>399</v>
-      </c>
-      <c r="C133" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="134" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C134" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="135" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B135" t="s">
+        <v>410</v>
+      </c>
+      <c r="C135" t="s">
         <v>411</v>
-      </c>
-      <c r="C135" t="s">
-        <v>412</v>
       </c>
     </row>
     <row r="136" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B136" t="s">
+        <v>521</v>
+      </c>
+      <c r="C136" t="s">
         <v>522</v>
-      </c>
-      <c r="C136" t="s">
-        <v>523</v>
       </c>
     </row>
     <row r="137" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B137" t="s">
+        <v>454</v>
+      </c>
+      <c r="C137" t="s">
         <v>455</v>
-      </c>
-      <c r="C137" t="s">
-        <v>456</v>
       </c>
     </row>
     <row r="138" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B138" t="s">
+        <v>368</v>
+      </c>
+      <c r="C138" t="s">
         <v>369</v>
-      </c>
-      <c r="C138" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="139" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B139" t="s">
+        <v>551</v>
+      </c>
+      <c r="C139" t="s">
         <v>552</v>
-      </c>
-      <c r="C139" t="s">
-        <v>553</v>
       </c>
     </row>
     <row r="140" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
+        <v>537</v>
+      </c>
+      <c r="C140" t="s">
         <v>538</v>
-      </c>
-      <c r="C140" t="s">
-        <v>539</v>
       </c>
     </row>
     <row r="141" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B141" t="s">
+        <v>317</v>
+      </c>
+      <c r="C141" t="s">
         <v>318</v>
-      </c>
-      <c r="C141" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="142" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B142" t="s">
+        <v>408</v>
+      </c>
+      <c r="C142" t="s">
         <v>409</v>
-      </c>
-      <c r="C142" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="143" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B143" t="s">
+        <v>277</v>
+      </c>
+      <c r="C143" t="s">
         <v>278</v>
-      </c>
-      <c r="C143" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="144" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B144" t="s">
+        <v>450</v>
+      </c>
+      <c r="C144" t="s">
         <v>451</v>
-      </c>
-      <c r="C144" t="s">
-        <v>452</v>
       </c>
     </row>
   </sheetData>
@@ -4541,7 +4744,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
@@ -4553,157 +4756,157 @@
   <sheetData>
     <row r="1" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C1" s="3"/>
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
+        <v>487</v>
+      </c>
+      <c r="C2" t="s">
         <v>488</v>
-      </c>
-      <c r="C2" t="s">
-        <v>489</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
+        <v>489</v>
+      </c>
+      <c r="C3" t="s">
         <v>490</v>
-      </c>
-      <c r="C3" t="s">
-        <v>491</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>461</v>
+      </c>
+      <c r="C4" t="s">
         <v>462</v>
-      </c>
-      <c r="C4" t="s">
-        <v>463</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="C5" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C6" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
+        <v>491</v>
+      </c>
+      <c r="C7" t="s">
         <v>492</v>
-      </c>
-      <c r="C7" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
+        <v>463</v>
+      </c>
+      <c r="C8" t="s">
         <v>464</v>
-      </c>
-      <c r="C8" t="s">
-        <v>465</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
+        <v>325</v>
+      </c>
+      <c r="C9" t="s">
         <v>326</v>
-      </c>
-      <c r="C9" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
+        <v>465</v>
+      </c>
+      <c r="C10" t="s">
         <v>466</v>
-      </c>
-      <c r="C10" t="s">
-        <v>467</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
+        <v>273</v>
+      </c>
+      <c r="C11" t="s">
         <v>274</v>
-      </c>
-      <c r="C11" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
+        <v>467</v>
+      </c>
+      <c r="C12" t="s">
         <v>468</v>
-      </c>
-      <c r="C12" t="s">
-        <v>469</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
+        <v>485</v>
+      </c>
+      <c r="C13" t="s">
         <v>486</v>
-      </c>
-      <c r="C13" t="s">
-        <v>487</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C14" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
+        <v>457</v>
+      </c>
+      <c r="C15" t="s">
         <v>458</v>
-      </c>
-      <c r="C15" t="s">
-        <v>459</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
+        <v>459</v>
+      </c>
+      <c r="C16" t="s">
         <v>460</v>
-      </c>
-      <c r="C16" t="s">
-        <v>461</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
+        <v>327</v>
+      </c>
+      <c r="C17" t="s">
         <v>328</v>
-      </c>
-      <c r="C17" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
+        <v>574</v>
+      </c>
+      <c r="C18" t="s">
         <v>575</v>
-      </c>
-      <c r="C18" t="s">
-        <v>576</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
+        <v>578</v>
+      </c>
+      <c r="C19" t="s">
         <v>579</v>
-      </c>
-      <c r="C19" t="s">
-        <v>580</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="C20" t="s">
         <v>11</v>
@@ -4722,49 +4925,276 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:C4"/>
+  <dimension ref="B1:C32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.5703125" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C1" s="3"/>
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>581</v>
+        <v>604</v>
       </c>
       <c r="C2" t="s">
-        <v>583</v>
+        <v>605</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>584</v>
+        <v>629</v>
       </c>
       <c r="C3" t="s">
-        <v>585</v>
+        <v>630</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>608</v>
+      </c>
+      <c r="C4" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>639</v>
+      </c>
+      <c r="C5" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>645</v>
+      </c>
+      <c r="C6" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>641</v>
+      </c>
+      <c r="C7" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>583</v>
+      </c>
+      <c r="C8" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>585</v>
+      </c>
+      <c r="C9" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>590</v>
+      </c>
+      <c r="C10" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>643</v>
+      </c>
+      <c r="C11" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>606</v>
+      </c>
+      <c r="C12" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>580</v>
+      </c>
+      <c r="C13" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>602</v>
+      </c>
+      <c r="C14" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>598</v>
+      </c>
+      <c r="C15" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>635</v>
+      </c>
+      <c r="C16" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>620</v>
+      </c>
+      <c r="C17" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>600</v>
+      </c>
+      <c r="C18" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>637</v>
+      </c>
+      <c r="C19" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>592</v>
+      </c>
+      <c r="C20" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>618</v>
+      </c>
+      <c r="C21" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
         <v>586</v>
       </c>
-      <c r="C4" t="s">
-        <v>586</v>
+      <c r="C22" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>622</v>
+      </c>
+      <c r="C23" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>631</v>
+      </c>
+      <c r="C24" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>633</v>
+      </c>
+      <c r="C25" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>594</v>
+      </c>
+      <c r="C26" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>616</v>
+      </c>
+      <c r="C27" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>624</v>
+      </c>
+      <c r="C28" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>612</v>
+      </c>
+      <c r="C29" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>610</v>
+      </c>
+      <c r="C30" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>611</v>
+      </c>
+      <c r="C31" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>627</v>
+      </c>
+      <c r="C32" t="s">
+        <v>628</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="B2:C32">
+    <sortCondition ref="B2"/>
+  </sortState>
   <mergeCells count="1">
     <mergeCell ref="B1:C1"/>
   </mergeCells>

</xml_diff>

<commit_message>
Traduzido ItWd_us.u16 até linha 450 (com dois itens da linha).
</commit_message>
<xml_diff>
--- a/glossario.xlsx
+++ b/glossario.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Diversos" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="652">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="661">
   <si>
     <t>Aerial Troop</t>
   </si>
@@ -53,9 +53,6 @@
     <t>Warp Key</t>
   </si>
   <si>
-    <t>Chave de Teletransporte</t>
-  </si>
-  <si>
     <t>Mechat</t>
   </si>
   <si>
@@ -1430,9 +1427,6 @@
     <t>King Ghost</t>
   </si>
   <si>
-    <t>Rei Fantasma</t>
-  </si>
-  <si>
     <t>Poo Snake</t>
   </si>
   <si>
@@ -1986,6 +1980,39 @@
   </si>
   <si>
     <t>Ataque Mágico +</t>
+  </si>
+  <si>
+    <t>Anchor</t>
+  </si>
+  <si>
+    <t>Âncora</t>
+  </si>
+  <si>
+    <t>Badge</t>
+  </si>
+  <si>
+    <t>Distintivo</t>
+  </si>
+  <si>
+    <t>Bellybutton Ring of Fire</t>
+  </si>
+  <si>
+    <t>Piercing de Fogo</t>
+  </si>
+  <si>
+    <t>Glowing Liquid</t>
+  </si>
+  <si>
+    <t>Líquido Brilhante</t>
+  </si>
+  <si>
+    <t>Rei Espectral</t>
+  </si>
+  <si>
+    <t>Shabby Book</t>
+  </si>
+  <si>
+    <t>Livro Deteriorado</t>
   </si>
 </sst>
 </file>
@@ -2328,10 +2355,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E42"/>
+  <dimension ref="B1:E41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2342,7 +2369,7 @@
   <sheetData>
     <row r="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C1" s="3"/>
     </row>
@@ -2356,34 +2383,34 @@
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
         <v>23</v>
-      </c>
-      <c r="C3" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>240</v>
+      </c>
+      <c r="C4" t="s">
         <v>241</v>
-      </c>
-      <c r="C4" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
         <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
         <v>21</v>
-      </c>
-      <c r="C6" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
@@ -2396,57 +2423,57 @@
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
         <v>19</v>
-      </c>
-      <c r="C8" t="s">
-        <v>20</v>
       </c>
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="C9" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
         <v>14</v>
-      </c>
-      <c r="C10" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
         <v>8</v>
-      </c>
-      <c r="C11" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
         <v>25</v>
-      </c>
-      <c r="C12" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
         <v>12</v>
       </c>
-      <c r="C13" t="s">
-        <v>13</v>
-      </c>
       <c r="D13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" t="s">
         <v>17</v>
-      </c>
-      <c r="E13" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
@@ -2462,19 +2489,11 @@
         <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D42" s="1"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D41" s="1"/>
     </row>
   </sheetData>
   <sortState ref="B2:C16">
@@ -2504,160 +2523,160 @@
   <sheetData>
     <row r="1" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C1" s="3"/>
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C2" t="s">
         <v>134</v>
-      </c>
-      <c r="C2" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" t="s">
         <v>74</v>
-      </c>
-      <c r="C3" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>139</v>
+      </c>
+      <c r="C4" t="s">
         <v>140</v>
-      </c>
-      <c r="C4" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
+        <v>153</v>
+      </c>
+      <c r="C5" t="s">
         <v>154</v>
-      </c>
-      <c r="C5" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6" t="s">
         <v>76</v>
-      </c>
-      <c r="C6" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" t="s">
         <v>76</v>
-      </c>
-      <c r="C7" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" t="s">
         <v>78</v>
-      </c>
-      <c r="C8" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" t="s">
         <v>78</v>
-      </c>
-      <c r="C9" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
+        <v>145</v>
+      </c>
+      <c r="C10" t="s">
         <v>146</v>
-      </c>
-      <c r="C10" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
+        <v>129</v>
+      </c>
+      <c r="C11" t="s">
         <v>130</v>
-      </c>
-      <c r="C11" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
+        <v>147</v>
+      </c>
+      <c r="C12" t="s">
         <v>148</v>
-      </c>
-      <c r="C12" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
+        <v>135</v>
+      </c>
+      <c r="C13" t="s">
         <v>136</v>
-      </c>
-      <c r="C13" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
+        <v>155</v>
+      </c>
+      <c r="C14" t="s">
         <v>156</v>
-      </c>
-      <c r="C14" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
+        <v>143</v>
+      </c>
+      <c r="C15" t="s">
         <v>144</v>
-      </c>
-      <c r="C15" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
+        <v>141</v>
+      </c>
+      <c r="C16" t="s">
         <v>142</v>
-      </c>
-      <c r="C16" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
+        <v>137</v>
+      </c>
+      <c r="C17" t="s">
         <v>138</v>
-      </c>
-      <c r="C17" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
+        <v>149</v>
+      </c>
+      <c r="C18" t="s">
         <v>150</v>
-      </c>
-      <c r="C18" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
+        <v>151</v>
+      </c>
+      <c r="C19" t="s">
         <v>152</v>
-      </c>
-      <c r="C19" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
+        <v>131</v>
+      </c>
+      <c r="C20" t="s">
         <v>132</v>
-      </c>
-      <c r="C20" t="s">
-        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -2675,7 +2694,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D28"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
@@ -2687,225 +2706,225 @@
   <sheetData>
     <row r="1" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C1" s="3"/>
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
         <v>27</v>
-      </c>
-      <c r="C2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" t="s">
         <v>29</v>
-      </c>
-      <c r="C3" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" t="s">
         <v>31</v>
-      </c>
-      <c r="C4" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" t="s">
         <v>39</v>
-      </c>
-      <c r="C8" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" t="s">
         <v>46</v>
-      </c>
-      <c r="C12" t="s">
-        <v>47</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" t="s">
         <v>48</v>
-      </c>
-      <c r="C13" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" t="s">
         <v>54</v>
-      </c>
-      <c r="C16" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" t="s">
         <v>56</v>
-      </c>
-      <c r="C17" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" t="s">
         <v>62</v>
-      </c>
-      <c r="C20" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" t="s">
         <v>64</v>
-      </c>
-      <c r="C21" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24" t="s">
         <v>70</v>
-      </c>
-      <c r="C24" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" t="s">
         <v>72</v>
-      </c>
-      <c r="C25" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="C26" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="C27" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="C28" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
   </sheetData>
@@ -2922,10 +2941,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G77"/>
+  <dimension ref="B1:G78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2936,93 +2955,93 @@
   <sheetData>
     <row r="1" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C1" s="3"/>
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>220</v>
+        <v>650</v>
       </c>
       <c r="C2" t="s">
-        <v>221</v>
+        <v>651</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>199</v>
+        <v>219</v>
       </c>
       <c r="C3" t="s">
-        <v>200</v>
+        <v>220</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>127</v>
+        <v>198</v>
       </c>
       <c r="C4" t="s">
-        <v>91</v>
+        <v>199</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>198</v>
+        <v>126</v>
       </c>
       <c r="C5" t="s">
-        <v>647</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>128</v>
+        <v>197</v>
       </c>
       <c r="C6" t="s">
-        <v>92</v>
+        <v>645</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
       <c r="C7" t="s">
-        <v>126</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>213</v>
+        <v>113</v>
       </c>
       <c r="C8" t="s">
-        <v>216</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C9" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C10" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>80</v>
+        <v>214</v>
       </c>
       <c r="C11" t="s">
-        <v>116</v>
+        <v>217</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C12" t="s">
         <v>115</v>
@@ -3030,201 +3049,201 @@
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C13" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C14" t="s">
-        <v>84</v>
+        <v>119</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C15" t="s">
-        <v>117</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C16" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>235</v>
+        <v>85</v>
       </c>
       <c r="C17" t="s">
-        <v>238</v>
-      </c>
-      <c r="F17" s="1"/>
+        <v>118</v>
+      </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C18" t="s">
-        <v>239</v>
-      </c>
+        <v>237</v>
+      </c>
+      <c r="F18" s="1"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C19" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>648</v>
+        <v>236</v>
       </c>
       <c r="C20" t="s">
-        <v>649</v>
+        <v>239</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>94</v>
+        <v>646</v>
       </c>
       <c r="C21" t="s">
-        <v>95</v>
+        <v>647</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>650</v>
+        <v>93</v>
       </c>
       <c r="C22" t="s">
-        <v>651</v>
+        <v>94</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>561</v>
+        <v>648</v>
       </c>
       <c r="C23" t="s">
-        <v>562</v>
-      </c>
-      <c r="G23" s="2"/>
+        <v>649</v>
+      </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>565</v>
+        <v>559</v>
       </c>
       <c r="C24" t="s">
-        <v>563</v>
-      </c>
+        <v>560</v>
+      </c>
+      <c r="G24" s="2"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="C25" t="s">
-        <v>572</v>
+        <v>561</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>170</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>171</v>
+        <v>562</v>
+      </c>
+      <c r="C26" t="s">
+        <v>570</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>87</v>
-      </c>
-      <c r="C27" t="s">
-        <v>88</v>
+        <v>169</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
+        <v>86</v>
+      </c>
+      <c r="C28" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>171</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>93</v>
-      </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>227</v>
-      </c>
-      <c r="C30" t="s">
-        <v>228</v>
+      <c r="B30" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>201</v>
+        <v>226</v>
       </c>
       <c r="C31" t="s">
-        <v>204</v>
+        <v>227</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C32" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C33" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>182</v>
+        <v>202</v>
       </c>
       <c r="C34" t="s">
-        <v>184</v>
+        <v>205</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
+        <v>181</v>
+      </c>
+      <c r="C35" t="s">
         <v>183</v>
-      </c>
-      <c r="C35" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>225</v>
+        <v>182</v>
       </c>
       <c r="C36" t="s">
-        <v>224</v>
+        <v>184</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="C37" t="s">
         <v>223</v>
@@ -3232,324 +3251,332 @@
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>566</v>
+        <v>221</v>
       </c>
       <c r="C38" t="s">
-        <v>567</v>
-      </c>
-      <c r="F38" s="1"/>
+        <v>222</v>
+      </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="C39" t="s">
-        <v>569</v>
-      </c>
+        <v>565</v>
+      </c>
+      <c r="F39" s="1"/>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="C40" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>164</v>
+        <v>568</v>
       </c>
       <c r="C41" t="s">
-        <v>168</v>
+        <v>569</v>
       </c>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C42" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C43" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>226</v>
+        <v>165</v>
       </c>
       <c r="C44" t="s">
-        <v>226</v>
+        <v>173</v>
       </c>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>96</v>
+        <v>225</v>
       </c>
       <c r="C45" t="s">
-        <v>99</v>
+        <v>225</v>
       </c>
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C46" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C47" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>186</v>
+        <v>97</v>
       </c>
       <c r="C48" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C49" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
+        <v>186</v>
+      </c>
+      <c r="C50" t="s">
         <v>188</v>
       </c>
-      <c r="C50" t="s">
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>187</v>
+      </c>
+      <c r="C51" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
+      <c r="C52" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
         <v>192</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="C53" s="2" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
+    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
         <v>193</v>
       </c>
-      <c r="C52" s="2" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
+      <c r="C54" t="s">
         <v>194</v>
       </c>
-      <c r="C53" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>99</v>
+      </c>
+      <c r="C55" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
         <v>100</v>
       </c>
-      <c r="C54" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
+      <c r="C56" t="s">
         <v>101</v>
       </c>
-      <c r="C55" t="s">
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>174</v>
+      </c>
+      <c r="C57" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>206</v>
+      </c>
+      <c r="C58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>207</v>
+      </c>
+      <c r="C59" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>208</v>
+      </c>
+      <c r="C60" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>88</v>
+      </c>
+      <c r="C61" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>594</v>
+      </c>
+      <c r="C62" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>361</v>
+      </c>
+      <c r="C63" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>175</v>
+      </c>
+      <c r="C64" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>176</v>
+      </c>
+      <c r="C65" t="s">
+        <v>179</v>
+      </c>
+      <c r="F65" s="1"/>
+    </row>
+    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>177</v>
+      </c>
+      <c r="C66" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>157</v>
+      </c>
+      <c r="C67" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>158</v>
+      </c>
+      <c r="C68" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>159</v>
+      </c>
+      <c r="C69" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="70" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B56" t="s">
-        <v>175</v>
-      </c>
-      <c r="C56" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
-        <v>207</v>
-      </c>
-      <c r="C57" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B58" t="s">
-        <v>208</v>
-      </c>
-      <c r="C58" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B59" t="s">
-        <v>209</v>
-      </c>
-      <c r="C59" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B60" t="s">
-        <v>89</v>
-      </c>
-      <c r="C60" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B61" t="s">
-        <v>596</v>
-      </c>
-      <c r="C61" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B62" t="s">
-        <v>362</v>
-      </c>
-      <c r="C62" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B63" t="s">
-        <v>176</v>
-      </c>
-      <c r="C63" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B64" t="s">
-        <v>177</v>
-      </c>
-      <c r="C64" t="s">
-        <v>180</v>
-      </c>
-      <c r="F64" s="1"/>
-    </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B65" t="s">
-        <v>178</v>
-      </c>
-      <c r="C65" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B66" t="s">
-        <v>158</v>
-      </c>
-      <c r="C66" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B67" t="s">
-        <v>159</v>
-      </c>
-      <c r="C67" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B68" t="s">
-        <v>160</v>
-      </c>
-      <c r="C68" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B69" t="s">
+      <c r="C70" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="71" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
         <v>103</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C71" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="72" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>104</v>
+      </c>
+      <c r="C72" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="73" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B70" t="s">
-        <v>104</v>
-      </c>
-      <c r="C70" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B71" t="s">
-        <v>105</v>
-      </c>
-      <c r="C71" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B72" t="s">
+      <c r="C73" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="74" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
         <v>107</v>
       </c>
-      <c r="C72" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="73" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B73" t="s">
+      <c r="C74" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="75" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
         <v>108</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C75" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="74" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B74" t="s">
-        <v>109</v>
-      </c>
-      <c r="C74" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="75" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B75" t="s">
+    <row r="76" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
+        <v>229</v>
+      </c>
+      <c r="C76" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="77" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
         <v>230</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C77" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="76" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B76" t="s">
-        <v>231</v>
-      </c>
-      <c r="C76" t="s">
+    <row r="78" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
+        <v>228</v>
+      </c>
+      <c r="C78" t="s">
         <v>233</v>
-      </c>
-    </row>
-    <row r="77" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B77" t="s">
-        <v>229</v>
-      </c>
-      <c r="C77" t="s">
-        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -3580,1152 +3607,1152 @@
   <sheetData>
     <row r="1" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C1" s="3"/>
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
+        <v>355</v>
+      </c>
+      <c r="C2" t="s">
         <v>356</v>
-      </c>
-      <c r="C2" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
+        <v>309</v>
+      </c>
+      <c r="C3" t="s">
         <v>310</v>
-      </c>
-      <c r="C3" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="C4" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="C5" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
+        <v>391</v>
+      </c>
+      <c r="C6" t="s">
         <v>392</v>
-      </c>
-      <c r="C6" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
+        <v>357</v>
+      </c>
+      <c r="C7" t="s">
         <v>358</v>
-      </c>
-      <c r="C7" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
+        <v>387</v>
+      </c>
+      <c r="C8" t="s">
         <v>388</v>
-      </c>
-      <c r="C8" t="s">
-        <v>389</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="C9" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
+        <v>294</v>
+      </c>
+      <c r="C11" t="s">
         <v>295</v>
-      </c>
-      <c r="C11" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
+        <v>252</v>
+      </c>
+      <c r="C12" t="s">
         <v>253</v>
-      </c>
-      <c r="C12" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="C13" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
+        <v>437</v>
+      </c>
+      <c r="C14" t="s">
         <v>438</v>
-      </c>
-      <c r="C14" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
+        <v>341</v>
+      </c>
+      <c r="C15" t="s">
         <v>342</v>
-      </c>
-      <c r="C15" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
+        <v>435</v>
+      </c>
+      <c r="C16" t="s">
         <v>436</v>
-      </c>
-      <c r="C16" t="s">
-        <v>437</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="C17" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
+        <v>417</v>
+      </c>
+      <c r="C18" t="s">
         <v>418</v>
-      </c>
-      <c r="C18" t="s">
-        <v>419</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="C20" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
+        <v>308</v>
+      </c>
+      <c r="C21" t="s">
         <v>309</v>
-      </c>
-      <c r="C21" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
+        <v>248</v>
+      </c>
+      <c r="C22" t="s">
         <v>249</v>
-      </c>
-      <c r="C22" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="C23" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
+        <v>399</v>
+      </c>
+      <c r="C24" t="s">
         <v>400</v>
-      </c>
-      <c r="C24" t="s">
-        <v>401</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
+        <v>280</v>
+      </c>
+      <c r="C25" t="s">
         <v>281</v>
-      </c>
-      <c r="C25" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="C26" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
+        <v>385</v>
+      </c>
+      <c r="C27" t="s">
         <v>386</v>
-      </c>
-      <c r="C27" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
+        <v>411</v>
+      </c>
+      <c r="C28" t="s">
         <v>412</v>
-      </c>
-      <c r="C28" t="s">
-        <v>413</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
+        <v>242</v>
+      </c>
+      <c r="C29" t="s">
         <v>243</v>
-      </c>
-      <c r="C29" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
+        <v>242</v>
+      </c>
+      <c r="C30" t="s">
         <v>243</v>
-      </c>
-      <c r="C30" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
+        <v>274</v>
+      </c>
+      <c r="C31" t="s">
         <v>275</v>
-      </c>
-      <c r="C31" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
+        <v>375</v>
+      </c>
+      <c r="C33" t="s">
         <v>376</v>
-      </c>
-      <c r="C33" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
+        <v>278</v>
+      </c>
+      <c r="C34" t="s">
         <v>279</v>
-      </c>
-      <c r="C34" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
+        <v>441</v>
+      </c>
+      <c r="C35" t="s">
         <v>442</v>
-      </c>
-      <c r="C35" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
+        <v>322</v>
+      </c>
+      <c r="C36" t="s">
         <v>323</v>
-      </c>
-      <c r="C36" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
+        <v>288</v>
+      </c>
+      <c r="C37" t="s">
         <v>289</v>
-      </c>
-      <c r="C37" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
+        <v>250</v>
+      </c>
+      <c r="C38" t="s">
         <v>251</v>
-      </c>
-      <c r="C38" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
+        <v>363</v>
+      </c>
+      <c r="C39" t="s">
         <v>364</v>
-      </c>
-      <c r="C39" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
+        <v>286</v>
+      </c>
+      <c r="C40" t="s">
         <v>287</v>
-      </c>
-      <c r="C40" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
+        <v>254</v>
+      </c>
+      <c r="C41" t="s">
         <v>255</v>
-      </c>
-      <c r="C41" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
+        <v>347</v>
+      </c>
+      <c r="C42" t="s">
         <v>348</v>
-      </c>
-      <c r="C42" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
+        <v>429</v>
+      </c>
+      <c r="C43" t="s">
         <v>430</v>
-      </c>
-      <c r="C43" t="s">
-        <v>431</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
+        <v>270</v>
+      </c>
+      <c r="C44" t="s">
         <v>271</v>
-      </c>
-      <c r="C44" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
+        <v>337</v>
+      </c>
+      <c r="C45" t="s">
         <v>338</v>
-      </c>
-      <c r="C45" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
+        <v>415</v>
+      </c>
+      <c r="C46" t="s">
         <v>416</v>
-      </c>
-      <c r="C46" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="C47" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
+        <v>445</v>
+      </c>
+      <c r="C48" t="s">
         <v>446</v>
-      </c>
-      <c r="C48" t="s">
-        <v>447</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
+        <v>292</v>
+      </c>
+      <c r="C49" t="s">
         <v>293</v>
-      </c>
-      <c r="C49" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
+        <v>433</v>
+      </c>
+      <c r="C50" t="s">
         <v>434</v>
-      </c>
-      <c r="C50" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
+        <v>393</v>
+      </c>
+      <c r="C51" t="s">
         <v>394</v>
-      </c>
-      <c r="C51" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
+        <v>371</v>
+      </c>
+      <c r="C52" t="s">
         <v>372</v>
-      </c>
-      <c r="C52" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="C53" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
+        <v>359</v>
+      </c>
+      <c r="C54" t="s">
         <v>360</v>
-      </c>
-      <c r="C54" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
+        <v>302</v>
+      </c>
+      <c r="C55" t="s">
         <v>303</v>
-      </c>
-      <c r="C55" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="C56" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
+        <v>343</v>
+      </c>
+      <c r="C57" t="s">
         <v>344</v>
-      </c>
-      <c r="C57" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
+        <v>447</v>
+      </c>
+      <c r="C58" t="s">
         <v>448</v>
-      </c>
-      <c r="C58" t="s">
-        <v>449</v>
       </c>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="C59" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
+        <v>381</v>
+      </c>
+      <c r="C60" t="s">
         <v>382</v>
-      </c>
-      <c r="C60" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
+        <v>439</v>
+      </c>
+      <c r="C61" t="s">
         <v>440</v>
-      </c>
-      <c r="C61" t="s">
-        <v>441</v>
       </c>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C62" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="63" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
+        <v>379</v>
+      </c>
+      <c r="C63" t="s">
         <v>380</v>
-      </c>
-      <c r="C63" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
+        <v>262</v>
+      </c>
+      <c r="C64" t="s">
         <v>263</v>
-      </c>
-      <c r="C64" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
+        <v>264</v>
+      </c>
+      <c r="C65" t="s">
         <v>265</v>
-      </c>
-      <c r="C65" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="C66" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="C67" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
+        <v>329</v>
+      </c>
+      <c r="C68" t="s">
         <v>330</v>
-      </c>
-      <c r="C68" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
+        <v>290</v>
+      </c>
+      <c r="C69" t="s">
         <v>291</v>
-      </c>
-      <c r="C69" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
+        <v>300</v>
+      </c>
+      <c r="C70" t="s">
         <v>301</v>
-      </c>
-      <c r="C70" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
+        <v>298</v>
+      </c>
+      <c r="C71" t="s">
         <v>299</v>
-      </c>
-      <c r="C71" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
+        <v>260</v>
+      </c>
+      <c r="C72" t="s">
         <v>261</v>
-      </c>
-      <c r="C72" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
+        <v>369</v>
+      </c>
+      <c r="C73" t="s">
         <v>370</v>
-      </c>
-      <c r="C73" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="74" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
+        <v>335</v>
+      </c>
+      <c r="C74" t="s">
         <v>336</v>
-      </c>
-      <c r="C74" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="75" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="C75" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="76" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
+        <v>256</v>
+      </c>
+      <c r="C76" t="s">
         <v>257</v>
-      </c>
-      <c r="C76" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="77" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
+        <v>296</v>
+      </c>
+      <c r="C77" t="s">
         <v>297</v>
-      </c>
-      <c r="C77" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="78" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="C78" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
     </row>
     <row r="79" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C79" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="80" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
+        <v>353</v>
+      </c>
+      <c r="C80" t="s">
         <v>354</v>
-      </c>
-      <c r="C80" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
+        <v>331</v>
+      </c>
+      <c r="C81" t="s">
         <v>332</v>
-      </c>
-      <c r="C81" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="82" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="C82" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="83" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
+        <v>427</v>
+      </c>
+      <c r="C83" t="s">
         <v>428</v>
-      </c>
-      <c r="C83" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="84" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="C84" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
     </row>
     <row r="85" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
+        <v>383</v>
+      </c>
+      <c r="C85" t="s">
         <v>384</v>
-      </c>
-      <c r="C85" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="86" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C86" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="87" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
+        <v>282</v>
+      </c>
+      <c r="C87" t="s">
         <v>283</v>
-      </c>
-      <c r="C87" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="88" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
+        <v>351</v>
+      </c>
+      <c r="C88" t="s">
         <v>352</v>
-      </c>
-      <c r="C88" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="89" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
+        <v>345</v>
+      </c>
+      <c r="C89" t="s">
         <v>346</v>
-      </c>
-      <c r="C89" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="90" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
+        <v>377</v>
+      </c>
+      <c r="C90" t="s">
         <v>378</v>
-      </c>
-      <c r="C90" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="91" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="C91" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="92" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
+        <v>268</v>
+      </c>
+      <c r="C92" t="s">
         <v>269</v>
-      </c>
-      <c r="C92" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="93" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
+        <v>310</v>
+      </c>
+      <c r="C93" t="s">
         <v>311</v>
-      </c>
-      <c r="C93" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="94" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
+        <v>311</v>
+      </c>
+      <c r="C94" t="s">
         <v>312</v>
-      </c>
-      <c r="C94" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="95" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
+        <v>246</v>
+      </c>
+      <c r="C95" t="s">
         <v>247</v>
-      </c>
-      <c r="C95" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="96" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
+        <v>431</v>
+      </c>
+      <c r="C96" t="s">
         <v>432</v>
-      </c>
-      <c r="C96" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="97" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="C97" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="98" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
+        <v>421</v>
+      </c>
+      <c r="C98" t="s">
         <v>422</v>
-      </c>
-      <c r="C98" t="s">
-        <v>423</v>
       </c>
     </row>
     <row r="99" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
     </row>
     <row r="100" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="C100" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
     </row>
     <row r="101" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
+        <v>333</v>
+      </c>
+      <c r="C101" t="s">
         <v>334</v>
-      </c>
-      <c r="C101" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="102" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
     </row>
     <row r="103" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
+        <v>306</v>
+      </c>
+      <c r="C103" t="s">
         <v>307</v>
-      </c>
-      <c r="C103" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="104" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C104" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="105" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="C105" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="106" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
+        <v>423</v>
+      </c>
+      <c r="C106" t="s">
         <v>424</v>
-      </c>
-      <c r="C106" t="s">
-        <v>425</v>
       </c>
     </row>
     <row r="107" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="C107" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
     </row>
     <row r="108" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
+        <v>395</v>
+      </c>
+      <c r="C108" t="s">
         <v>396</v>
-      </c>
-      <c r="C108" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="109" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
+        <v>349</v>
+      </c>
+      <c r="C109" t="s">
         <v>350</v>
-      </c>
-      <c r="C109" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="110" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
+        <v>320</v>
+      </c>
+      <c r="C110" t="s">
         <v>321</v>
-      </c>
-      <c r="C110" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="111" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
     </row>
     <row r="112" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C112" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="113" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
+        <v>401</v>
+      </c>
+      <c r="C113" s="2" t="s">
         <v>402</v>
-      </c>
-      <c r="C113" s="2" t="s">
-        <v>403</v>
       </c>
     </row>
     <row r="114" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
+        <v>443</v>
+      </c>
+      <c r="C114" t="s">
         <v>444</v>
-      </c>
-      <c r="C114" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="115" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
+        <v>266</v>
+      </c>
+      <c r="C115" t="s">
         <v>267</v>
-      </c>
-      <c r="C115" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="116" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
+        <v>318</v>
+      </c>
+      <c r="C116" t="s">
         <v>319</v>
-      </c>
-      <c r="C116" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="117" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
+        <v>413</v>
+      </c>
+      <c r="C117" t="s">
         <v>414</v>
-      </c>
-      <c r="C117" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="118" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="C118" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
     </row>
     <row r="119" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C119" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="120" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
+        <v>373</v>
+      </c>
+      <c r="C120" t="s">
         <v>374</v>
-      </c>
-      <c r="C120" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="121" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="C121" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="122" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
+        <v>284</v>
+      </c>
+      <c r="C122" t="s">
         <v>285</v>
-      </c>
-      <c r="C122" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="123" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
+        <v>258</v>
+      </c>
+      <c r="C123" t="s">
         <v>259</v>
-      </c>
-      <c r="C123" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="124" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="C124" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="125" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
+        <v>425</v>
+      </c>
+      <c r="C125" t="s">
         <v>426</v>
-      </c>
-      <c r="C125" t="s">
-        <v>427</v>
       </c>
     </row>
     <row r="126" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="C126" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="127" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
+        <v>339</v>
+      </c>
+      <c r="C127" t="s">
         <v>340</v>
-      </c>
-      <c r="C127" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="128" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
+        <v>244</v>
+      </c>
+      <c r="C128" t="s">
         <v>245</v>
-      </c>
-      <c r="C128" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="129" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
+        <v>304</v>
+      </c>
+      <c r="C129" t="s">
         <v>305</v>
-      </c>
-      <c r="C129" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="130" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B130" t="s">
+        <v>451</v>
+      </c>
+      <c r="C130" t="s">
         <v>452</v>
-      </c>
-      <c r="C130" t="s">
-        <v>453</v>
       </c>
     </row>
     <row r="131" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
+        <v>365</v>
+      </c>
+      <c r="C131" t="s">
         <v>366</v>
-      </c>
-      <c r="C131" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="132" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="C132" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="133" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B133" t="s">
+        <v>397</v>
+      </c>
+      <c r="C133" t="s">
         <v>398</v>
-      </c>
-      <c r="C133" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="134" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="C134" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="135" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B135" t="s">
+        <v>409</v>
+      </c>
+      <c r="C135" t="s">
         <v>410</v>
-      </c>
-      <c r="C135" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="136" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B136" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="C136" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="137" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B137" t="s">
+        <v>453</v>
+      </c>
+      <c r="C137" t="s">
         <v>454</v>
-      </c>
-      <c r="C137" t="s">
-        <v>455</v>
       </c>
     </row>
     <row r="138" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B138" t="s">
+        <v>367</v>
+      </c>
+      <c r="C138" t="s">
         <v>368</v>
-      </c>
-      <c r="C138" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="139" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B139" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="C139" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="140" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="C140" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
     </row>
     <row r="141" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B141" t="s">
+        <v>316</v>
+      </c>
+      <c r="C141" t="s">
         <v>317</v>
-      </c>
-      <c r="C141" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="142" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B142" t="s">
+        <v>407</v>
+      </c>
+      <c r="C142" t="s">
         <v>408</v>
-      </c>
-      <c r="C142" t="s">
-        <v>409</v>
       </c>
     </row>
     <row r="143" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B143" t="s">
+        <v>276</v>
+      </c>
+      <c r="C143" t="s">
         <v>277</v>
-      </c>
-      <c r="C143" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="144" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B144" t="s">
+        <v>449</v>
+      </c>
+      <c r="C144" t="s">
         <v>450</v>
-      </c>
-      <c r="C144" t="s">
-        <v>451</v>
       </c>
     </row>
   </sheetData>
@@ -4745,7 +4772,7 @@
   <dimension ref="B1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="B21" sqref="B21:C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4756,160 +4783,160 @@
   <sheetData>
     <row r="1" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C1" s="3"/>
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="C2" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="C3" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>460</v>
+      </c>
+      <c r="C4" t="s">
         <v>461</v>
-      </c>
-      <c r="C4" t="s">
-        <v>462</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="C5" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C6" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="C7" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
+        <v>462</v>
+      </c>
+      <c r="C8" t="s">
         <v>463</v>
-      </c>
-      <c r="C8" t="s">
-        <v>464</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
+        <v>324</v>
+      </c>
+      <c r="C9" t="s">
         <v>325</v>
-      </c>
-      <c r="C9" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C10" t="s">
-        <v>466</v>
+        <v>658</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
+        <v>272</v>
+      </c>
+      <c r="C11" t="s">
         <v>273</v>
-      </c>
-      <c r="C11" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="C12" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="C13" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C14" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
+        <v>456</v>
+      </c>
+      <c r="C15" t="s">
         <v>457</v>
-      </c>
-      <c r="C15" t="s">
-        <v>458</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
+        <v>458</v>
+      </c>
+      <c r="C16" t="s">
         <v>459</v>
-      </c>
-      <c r="C16" t="s">
-        <v>460</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
+        <v>326</v>
+      </c>
+      <c r="C17" t="s">
         <v>327</v>
-      </c>
-      <c r="C17" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="C18" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="C19" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="C20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -4925,10 +4952,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:C32"/>
+  <dimension ref="B1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4939,260 +4966,292 @@
   <sheetData>
     <row r="1" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="C1" s="3"/>
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="C2" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="C3" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="C4" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>639</v>
+        <v>652</v>
       </c>
       <c r="C5" t="s">
-        <v>640</v>
+        <v>653</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>645</v>
+        <v>637</v>
       </c>
       <c r="C6" t="s">
-        <v>646</v>
+        <v>638</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>641</v>
+        <v>654</v>
       </c>
       <c r="C7" t="s">
-        <v>642</v>
+        <v>655</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>583</v>
+        <v>643</v>
       </c>
       <c r="C8" t="s">
-        <v>584</v>
+        <v>644</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>585</v>
+        <v>639</v>
       </c>
       <c r="C9" t="s">
-        <v>585</v>
+        <v>640</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>590</v>
+        <v>581</v>
       </c>
       <c r="C10" t="s">
-        <v>591</v>
+        <v>582</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>643</v>
+        <v>583</v>
       </c>
       <c r="C11" t="s">
-        <v>644</v>
+        <v>583</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>606</v>
+        <v>588</v>
       </c>
       <c r="C12" t="s">
-        <v>607</v>
+        <v>589</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>580</v>
+        <v>656</v>
       </c>
       <c r="C13" t="s">
-        <v>582</v>
+        <v>657</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>602</v>
+        <v>641</v>
       </c>
       <c r="C14" t="s">
-        <v>603</v>
+        <v>642</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>598</v>
+        <v>604</v>
       </c>
       <c r="C15" t="s">
-        <v>599</v>
+        <v>605</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>635</v>
+        <v>578</v>
       </c>
       <c r="C16" t="s">
-        <v>636</v>
+        <v>580</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>620</v>
+        <v>600</v>
       </c>
       <c r="C17" t="s">
-        <v>621</v>
+        <v>601</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="C18" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="C19" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>592</v>
+        <v>618</v>
       </c>
       <c r="C20" t="s">
-        <v>593</v>
+        <v>619</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>618</v>
+        <v>598</v>
       </c>
       <c r="C21" t="s">
-        <v>619</v>
+        <v>599</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>586</v>
+        <v>635</v>
       </c>
       <c r="C22" t="s">
-        <v>626</v>
+        <v>636</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>622</v>
+        <v>590</v>
       </c>
       <c r="C23" t="s">
-        <v>623</v>
+        <v>591</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>631</v>
+        <v>616</v>
       </c>
       <c r="C24" t="s">
-        <v>632</v>
+        <v>617</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>633</v>
+        <v>584</v>
       </c>
       <c r="C25" t="s">
-        <v>634</v>
+        <v>624</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>594</v>
+        <v>620</v>
       </c>
       <c r="C26" t="s">
-        <v>595</v>
+        <v>621</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>616</v>
+        <v>659</v>
       </c>
       <c r="C27" t="s">
-        <v>617</v>
+        <v>660</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>624</v>
+        <v>629</v>
       </c>
       <c r="C28" t="s">
-        <v>625</v>
+        <v>630</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>612</v>
+        <v>631</v>
       </c>
       <c r="C29" t="s">
-        <v>615</v>
+        <v>632</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>610</v>
+        <v>592</v>
       </c>
       <c r="C30" t="s">
-        <v>614</v>
+        <v>593</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>611</v>
+        <v>614</v>
       </c>
       <c r="C31" t="s">
-        <v>613</v>
+        <v>615</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>627</v>
+        <v>622</v>
       </c>
       <c r="C32" t="s">
-        <v>628</v>
+        <v>623</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>610</v>
+      </c>
+      <c r="C33" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>608</v>
+      </c>
+      <c r="C34" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>609</v>
+      </c>
+      <c r="C35" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>625</v>
+      </c>
+      <c r="C36" t="s">
+        <v>626</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="B2:C32">
+  <sortState ref="B2:C36">
     <sortCondition ref="B2"/>
   </sortState>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Concluída a tradução da primeira e terceira coluna do arquivo item. Falta agora a descrição completa.
</commit_message>
<xml_diff>
--- a/glossario.xlsx
+++ b/glossario.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Diversos" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="661">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="724">
   <si>
     <t>Aerial Troop</t>
   </si>
@@ -2013,6 +2013,195 @@
   </si>
   <si>
     <t>Livro Deteriorado</t>
+  </si>
+  <si>
+    <t>Lock-On Upgrade Part A</t>
+  </si>
+  <si>
+    <t>Missile Upgrade Part A</t>
+  </si>
+  <si>
+    <t>Peça A para melhoria de mísseis</t>
+  </si>
+  <si>
+    <t>Coating Part A</t>
+  </si>
+  <si>
+    <t>Peça A para revestimento</t>
+  </si>
+  <si>
+    <t>Magic Life-Crusher Bracelet</t>
+  </si>
+  <si>
+    <t>Pulseira Quebra Vida Mágica</t>
+  </si>
+  <si>
+    <t>Heatsink Parts</t>
+  </si>
+  <si>
+    <t>Peças Refrigeradoras</t>
+  </si>
+  <si>
+    <t>Creature Compendium</t>
+  </si>
+  <si>
+    <t>Compêndio de Criaturas</t>
+  </si>
+  <si>
+    <t>Belt of Hermes</t>
+  </si>
+  <si>
+    <t>Cinturão de Hermes</t>
+  </si>
+  <si>
+    <t>Belt</t>
+  </si>
+  <si>
+    <t>Cinturão</t>
+  </si>
+  <si>
+    <t>Earring</t>
+  </si>
+  <si>
+    <t>Brinco</t>
+  </si>
+  <si>
+    <t>Copper Earring</t>
+  </si>
+  <si>
+    <t>Brinco de Cobre</t>
+  </si>
+  <si>
+    <t>Bow Tie</t>
+  </si>
+  <si>
+    <t>Gravata Borboleta</t>
+  </si>
+  <si>
+    <t>Eyepatch</t>
+  </si>
+  <si>
+    <t>Tapa-Olho</t>
+  </si>
+  <si>
+    <t>Ribbon</t>
+  </si>
+  <si>
+    <t>Laço</t>
+  </si>
+  <si>
+    <t>Collar</t>
+  </si>
+  <si>
+    <t>Colar</t>
+  </si>
+  <si>
+    <t>Scarf</t>
+  </si>
+  <si>
+    <t>Cachecol</t>
+  </si>
+  <si>
+    <t>Kimono Sash</t>
+  </si>
+  <si>
+    <t>Faixa de quimono</t>
+  </si>
+  <si>
+    <t>Stomach-Band</t>
+  </si>
+  <si>
+    <t>Faixa de Barriga</t>
+  </si>
+  <si>
+    <t>Necklace</t>
+  </si>
+  <si>
+    <t>Shadowstep Shoes</t>
+  </si>
+  <si>
+    <t>Sapatos de Introspecção</t>
+  </si>
+  <si>
+    <t>Bracelet</t>
+  </si>
+  <si>
+    <t>Pulseira</t>
+  </si>
+  <si>
+    <t>Flame Bracelet</t>
+  </si>
+  <si>
+    <t>Pulseira Flamejante</t>
+  </si>
+  <si>
+    <t>Gravitic Bracelet</t>
+  </si>
+  <si>
+    <t>Pulseira Gravitacional</t>
+  </si>
+  <si>
+    <t>Renew Bracelet</t>
+  </si>
+  <si>
+    <t>Pulseira Vital</t>
+  </si>
+  <si>
+    <t>Ordeal Necklace</t>
+  </si>
+  <si>
+    <t>Colar de Ordeal</t>
+  </si>
+  <si>
+    <t>Kerchief</t>
+  </si>
+  <si>
+    <t>Lenço</t>
+  </si>
+  <si>
+    <t>Eternity Earring</t>
+  </si>
+  <si>
+    <t>Brinco Eterno</t>
+  </si>
+  <si>
+    <t>Acorn Shoes</t>
+  </si>
+  <si>
+    <t>Sapato de Bolotas</t>
+  </si>
+  <si>
+    <t>Flip-Flops</t>
+  </si>
+  <si>
+    <t>Chinelos</t>
+  </si>
+  <si>
+    <t>Cross Trainers</t>
+  </si>
+  <si>
+    <t>Desportivas</t>
+  </si>
+  <si>
+    <t>Flying Fortress</t>
+  </si>
+  <si>
+    <t>Fortaleza Flutuante</t>
+  </si>
+  <si>
+    <t>Underwater Cave</t>
+  </si>
+  <si>
+    <t>Caverna Submarina</t>
+  </si>
+  <si>
+    <t>Peça A para melhoria de mira</t>
+  </si>
+  <si>
+    <t>Heaving Herb</t>
+  </si>
+  <si>
+    <t>Erva Anti-Vômito</t>
   </si>
 </sst>
 </file>
@@ -2692,10 +2881,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D28"/>
+  <dimension ref="B1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2776,147 +2965,147 @@
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>40</v>
+        <v>717</v>
       </c>
       <c r="C10" t="s">
-        <v>43</v>
+        <v>718</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C14" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C16" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C17" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C18" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>61</v>
+        <v>494</v>
       </c>
       <c r="C20" t="s">
-        <v>62</v>
+        <v>495</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C21" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C22" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C23" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C24" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C25" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>492</v>
+        <v>69</v>
       </c>
       <c r="C26" t="s">
-        <v>493</v>
+        <v>70</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>494</v>
+        <v>719</v>
       </c>
       <c r="C27" t="s">
-        <v>495</v>
+        <v>720</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
@@ -2927,8 +3116,24 @@
         <v>497</v>
       </c>
     </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>492</v>
+      </c>
+      <c r="C29" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>71</v>
+      </c>
+      <c r="C30" t="s">
+        <v>72</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="B2:C25">
+  <sortState ref="B2:C30">
     <sortCondition ref="B2"/>
   </sortState>
   <mergeCells count="1">
@@ -2943,8 +3148,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G78"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4952,10 +5157,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:C36"/>
+  <dimension ref="B1:G66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4972,291 +5177,533 @@
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>602</v>
+        <v>711</v>
       </c>
       <c r="C2" t="s">
-        <v>603</v>
+        <v>712</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>627</v>
+        <v>602</v>
       </c>
       <c r="C3" t="s">
-        <v>628</v>
+        <v>603</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>606</v>
+        <v>627</v>
       </c>
       <c r="C4" t="s">
-        <v>607</v>
+        <v>628</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>652</v>
+        <v>606</v>
       </c>
       <c r="C5" t="s">
-        <v>653</v>
+        <v>607</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>637</v>
+        <v>652</v>
       </c>
       <c r="C6" t="s">
-        <v>638</v>
+        <v>653</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>654</v>
+        <v>637</v>
       </c>
       <c r="C7" t="s">
-        <v>655</v>
+        <v>638</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>643</v>
+        <v>654</v>
       </c>
       <c r="C8" t="s">
-        <v>644</v>
+        <v>655</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>639</v>
+        <v>674</v>
       </c>
       <c r="C9" t="s">
-        <v>640</v>
+        <v>675</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>581</v>
+        <v>672</v>
       </c>
       <c r="C10" t="s">
-        <v>582</v>
+        <v>673</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>583</v>
+        <v>643</v>
       </c>
       <c r="C11" t="s">
-        <v>583</v>
+        <v>644</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>588</v>
+        <v>680</v>
       </c>
       <c r="C12" t="s">
-        <v>589</v>
+        <v>681</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>656</v>
-      </c>
-      <c r="C13" t="s">
-        <v>657</v>
+        <v>697</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>698</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>641</v>
+        <v>664</v>
       </c>
       <c r="C14" t="s">
-        <v>642</v>
+        <v>665</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>604</v>
+        <v>686</v>
       </c>
       <c r="C15" t="s">
-        <v>605</v>
+        <v>687</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>578</v>
+        <v>678</v>
       </c>
       <c r="C16" t="s">
-        <v>580</v>
+        <v>679</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>600</v>
+        <v>670</v>
       </c>
       <c r="C17" t="s">
-        <v>601</v>
+        <v>671</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>596</v>
+        <v>715</v>
       </c>
       <c r="C18" t="s">
-        <v>597</v>
+        <v>716</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>633</v>
+        <v>639</v>
       </c>
       <c r="C19" t="s">
-        <v>634</v>
+        <v>640</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>618</v>
+        <v>581</v>
       </c>
       <c r="C20" t="s">
-        <v>619</v>
+        <v>582</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>598</v>
+        <v>676</v>
       </c>
       <c r="C21" t="s">
-        <v>599</v>
+        <v>677</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>635</v>
+        <v>583</v>
       </c>
       <c r="C22" t="s">
-        <v>636</v>
+        <v>583</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>590</v>
+        <v>709</v>
       </c>
       <c r="C23" t="s">
-        <v>591</v>
+        <v>710</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>616</v>
+        <v>682</v>
       </c>
       <c r="C24" t="s">
-        <v>617</v>
+        <v>683</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>584</v>
+        <v>699</v>
       </c>
       <c r="C25" t="s">
-        <v>624</v>
+        <v>700</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>620</v>
+        <v>588</v>
       </c>
       <c r="C26" t="s">
-        <v>621</v>
+        <v>589</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>659</v>
+        <v>713</v>
       </c>
       <c r="C27" t="s">
-        <v>660</v>
+        <v>714</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>629</v>
+        <v>656</v>
       </c>
       <c r="C28" t="s">
-        <v>630</v>
+        <v>657</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>631</v>
+        <v>701</v>
       </c>
       <c r="C29" t="s">
-        <v>632</v>
+        <v>702</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>592</v>
+        <v>668</v>
       </c>
       <c r="C30" t="s">
-        <v>593</v>
+        <v>669</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>614</v>
+        <v>722</v>
       </c>
       <c r="C31" t="s">
-        <v>615</v>
+        <v>723</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
+        <v>641</v>
+      </c>
+      <c r="C32" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>604</v>
+      </c>
+      <c r="C33" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>707</v>
+      </c>
+      <c r="C34" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>690</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>661</v>
+      </c>
+      <c r="C36" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>666</v>
+      </c>
+      <c r="C37" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>578</v>
+      </c>
+      <c r="C38" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>600</v>
+      </c>
+      <c r="C39" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>662</v>
+      </c>
+      <c r="C40" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>596</v>
+      </c>
+      <c r="C41" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>633</v>
+      </c>
+      <c r="C42" t="s">
+        <v>634</v>
+      </c>
+      <c r="G42" s="2"/>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>618</v>
+      </c>
+      <c r="C43" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>694</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>598</v>
+      </c>
+      <c r="C45" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>705</v>
+      </c>
+      <c r="C46" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>635</v>
+      </c>
+      <c r="C47" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>590</v>
+      </c>
+      <c r="C48" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>616</v>
+      </c>
+      <c r="C49" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>584</v>
+      </c>
+      <c r="C50" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>703</v>
+      </c>
+      <c r="C51" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>620</v>
+      </c>
+      <c r="C52" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>684</v>
+      </c>
+      <c r="C53" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>688</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>659</v>
+      </c>
+      <c r="C55" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>695</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>629</v>
+      </c>
+      <c r="C57" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>631</v>
+      </c>
+      <c r="C58" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>592</v>
+      </c>
+      <c r="C59" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>614</v>
+      </c>
+      <c r="C60" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>692</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
         <v>622</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C62" t="s">
         <v>623</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
+    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
         <v>610</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C63" t="s">
         <v>613</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
+    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
         <v>608</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C64" t="s">
         <v>612</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
+    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
         <v>609</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C65" t="s">
         <v>611</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
+    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
         <v>625</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C66" t="s">
         <v>626</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="B2:C36">
+  <sortState ref="B2:C66">
     <sortCondition ref="B2"/>
   </sortState>
   <mergeCells count="1">
     <mergeCell ref="B1:C1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>